<commit_message>
date fix for canada university export
prefers 2015 (within range of protests) to most recent year 2020
</commit_message>
<xml_diff>
--- a/tasks/university_covariates/hand/canadian_universities.xlsx
+++ b/tasks/university_covariates/hand/canadian_universities.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G140"/>
+  <dimension ref="A1:H140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -394,20 +394,25 @@
           <t>enrollment_count</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>(ACAD)</t>
+          <t>Acadia University</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>IAU-000812-1</t>
+          <t>IAU-000076-1</t>
         </is>
       </c>
       <c r="C2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -419,18 +424,21 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1298</v>
+        <v>3869</v>
+      </c>
+      <c r="H2">
+        <v>2015</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>(Ai Vancouver)</t>
+          <t>Alberta College Of Art And Design</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>IAU-022835-1</t>
+          <t>IAU-000812-1</t>
         </is>
       </c>
       <c r="C3" t="b">
@@ -440,24 +448,27 @@
         <v>1</v>
       </c>
       <c r="E3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>1848</v>
+        <v>1247</v>
+      </c>
+      <c r="H3">
+        <v>2015</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>(BCIT)</t>
+          <t>Algonquin College</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>IAU-001770-1</t>
+          <t>IAU-000830-1</t>
         </is>
       </c>
       <c r="C4" t="b">
@@ -467,24 +478,27 @@
         <v>1</v>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>45684</v>
+        <v>19000</v>
+      </c>
+      <c r="H4">
+        <v>2015</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>(BU)</t>
+          <t>Ambrose University</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>IAU-001747-1</t>
+          <t>IAU-000890-1</t>
         </is>
       </c>
       <c r="C5" t="b">
@@ -497,48 +511,54 @@
         <v>1</v>
       </c>
       <c r="F5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>3303</v>
+        <v>842</v>
+      </c>
+      <c r="H5">
+        <v>2015</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>(CMCC)</t>
+          <t>Athabasca University</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>IAU-001954-1</t>
+          <t>IAU-001258-1</t>
         </is>
       </c>
       <c r="C6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>800</v>
+        <v>40108</v>
+      </c>
+      <c r="H6">
+        <v>2015</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>(CMU)</t>
+          <t>Kingswood University</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>IAU-001955-1</t>
+          <t>IAU-001620-1</t>
         </is>
       </c>
       <c r="C7" t="b">
@@ -554,45 +574,51 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>1692</v>
+        <v>300</v>
+      </c>
+      <c r="H7">
+        <v>2015</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>(GBC)</t>
+          <t>Bishop'S University</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>IAU-006615-1</t>
+          <t>IAU-001686-1</t>
         </is>
       </c>
       <c r="C8" t="b">
         <v>0</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>35893</v>
+        <v>2788</v>
+      </c>
+      <c r="H8">
+        <v>2015</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>(Huron)</t>
+          <t>Booth University College</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>IAU-020629-007657-1</t>
+          <t>IAU-001724-1</t>
         </is>
       </c>
       <c r="C9" t="b">
@@ -602,24 +628,27 @@
         <v>1</v>
       </c>
       <c r="E9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>40235</v>
+        <v>248</v>
+      </c>
+      <c r="H9">
+        <v>2015</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>(MHC)</t>
+          <t>Brandon University</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>IAU-011516-1</t>
+          <t>IAU-001747-1</t>
         </is>
       </c>
       <c r="C10" t="b">
@@ -629,24 +658,27 @@
         <v>1</v>
       </c>
       <c r="E10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>2477</v>
+        <v>3069</v>
+      </c>
+      <c r="H10">
+        <v>2015</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>(NAIT)</t>
+          <t>Brescia University College</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>IAU-012815-1</t>
+          <t>IAU-001755-1</t>
         </is>
       </c>
       <c r="C11" t="b">
@@ -656,24 +688,27 @@
         <v>1</v>
       </c>
       <c r="E11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>22180</v>
+        <v>1255</v>
+      </c>
+      <c r="H11">
+        <v>2015</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>(OCAD)</t>
+          <t>British Columbia Institute Of Technology</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>IAU-013094-1</t>
+          <t>IAU-001770-1</t>
         </is>
       </c>
       <c r="C12" t="b">
@@ -689,39 +724,51 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>5716</v>
+        <v>40178</v>
+      </c>
+      <c r="H12">
+        <v>2015</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>(OCCI)</t>
+          <t>Brock University</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>IAU-013054-1</t>
+          <t>IAU-001778-1</t>
         </is>
       </c>
       <c r="C13" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>3800</v>
+        <v>18706</v>
+      </c>
+      <c r="H13">
+        <v>2015</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>(OUC)</t>
+          <t>Camosun College</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>IAU-013031-1</t>
+          <t>IAU-001940-1</t>
         </is>
       </c>
       <c r="C14" t="b">
@@ -737,45 +784,51 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>8278</v>
+        <v>8612</v>
+      </c>
+      <c r="H14">
+        <v>2015</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>(RDC)</t>
+          <t>Canadian Memorial Chiropractic College</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>IAU-013935-1</t>
+          <t>IAU-001954-1</t>
         </is>
       </c>
       <c r="C15" t="b">
         <v>0</v>
       </c>
       <c r="D15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
       </c>
       <c r="F15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>8821</v>
+        <v>703</v>
+      </c>
+      <c r="H15">
+        <v>2015</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>(SJU)</t>
+          <t>Canadian Mennonite University</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>IAU-015746-1</t>
+          <t>IAU-001955-1</t>
         </is>
       </c>
       <c r="C16" t="b">
@@ -788,21 +841,24 @@
         <v>1</v>
       </c>
       <c r="F16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16">
-        <v>1019</v>
+        <v>1488</v>
+      </c>
+      <c r="H16">
+        <v>2015</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>(SLC)</t>
+          <t>Burman University</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>IAU-015759-1</t>
+          <t>IAU-001956-1</t>
         </is>
       </c>
       <c r="C17" t="b">
@@ -818,45 +874,45 @@
         <v>1</v>
       </c>
       <c r="G17">
-        <v>6700</v>
+        <v>421</v>
+      </c>
+      <c r="H17">
+        <v>2015</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>(SSU)</t>
+          <t>Cape Breton University</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>IAU-015791-1</t>
+          <t>IAU-001969-1</t>
         </is>
       </c>
       <c r="C18" t="b">
         <v>0</v>
       </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" t="b">
-        <v>1</v>
-      </c>
       <c r="F18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>91</v>
+        <v>3500</v>
+      </c>
+      <c r="H18">
+        <v>2015</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>(TRU)</t>
+          <t>Capilano University</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>IAU-016643-1</t>
+          <t>IAU-001973-1</t>
         </is>
       </c>
       <c r="C19" t="b">
@@ -866,24 +922,27 @@
         <v>1</v>
       </c>
       <c r="E19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
       </c>
       <c r="G19">
-        <v>9120</v>
+        <v>6920</v>
+      </c>
+      <c r="H19">
+        <v>2015</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>(U of A)</t>
+          <t>Carleton University</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>IAU-020010-1</t>
+          <t>IAU-001997-1</t>
         </is>
       </c>
       <c r="C20" t="b">
@@ -897,75 +956,87 @@
       </c>
       <c r="F20" t="b">
         <v>0</v>
+      </c>
+      <c r="G20">
+        <v>27883</v>
+      </c>
+      <c r="H20">
+        <v>2015</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>(U of C)</t>
+          <t>Centennial College</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>IAU-020053-1</t>
+          <t>IAU-002055-1</t>
         </is>
       </c>
       <c r="C21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="b">
         <v>1</v>
       </c>
       <c r="E21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
       </c>
       <c r="G21">
-        <v>31857</v>
+        <v>22866</v>
+      </c>
+      <c r="H21">
+        <v>2015</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>(U of G)</t>
+          <t>La Cité College Of Applied Arts And Technology</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>IAU-020173-1</t>
+          <t>IAU-002993-1</t>
         </is>
       </c>
       <c r="C22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" t="b">
         <v>1</v>
       </c>
       <c r="E22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>28430</v>
+        <v>3387</v>
+      </c>
+      <c r="H22">
+        <v>2015</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>(U of L)</t>
+          <t>University Of Saint-Boniface</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>IAU-020225-1</t>
+          <t>IAU-003046-1</t>
         </is>
       </c>
       <c r="C23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" t="b">
         <v>1</v>
@@ -977,18 +1048,21 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <v>9111</v>
+        <v>1124</v>
+      </c>
+      <c r="H23">
+        <v>2015</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>(U of R)</t>
+          <t>Dominican University College</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>IAU-020447-1</t>
+          <t>IAU-003047-1</t>
         </is>
       </c>
       <c r="C24" t="b">
@@ -1001,21 +1075,24 @@
         <v>1</v>
       </c>
       <c r="F24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>16048</v>
+        <v>405</v>
+      </c>
+      <c r="H24">
+        <v>2015</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>(U of S)</t>
+          <t>Concordia University</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>IAU-020476-1</t>
+          <t>IAU-003125-1</t>
         </is>
       </c>
       <c r="C25" t="b">
@@ -1031,22 +1108,25 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>24345</v>
+        <v>44568</v>
+      </c>
+      <c r="H25">
+        <v>2015</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>(U of T)</t>
+          <t>Concordia University Of Edmonton</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>IAU-020599-1</t>
+          <t>IAU-003129-1</t>
         </is>
       </c>
       <c r="C26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" t="b">
         <v>1</v>
@@ -1058,45 +1138,51 @@
         <v>1</v>
       </c>
       <c r="G26">
-        <v>70028</v>
+        <v>1986</v>
+      </c>
+      <c r="H26">
+        <v>2015</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>(UBC)</t>
+          <t>Conestoga College</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>IAU-016562-1</t>
+          <t>IAU-003135-1</t>
         </is>
       </c>
       <c r="C27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" t="b">
         <v>1</v>
       </c>
       <c r="E27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
       </c>
       <c r="G27">
-        <v>64378</v>
+        <v>11000</v>
+      </c>
+      <c r="H27">
+        <v>2015</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>(UCN)</t>
+          <t>Crandall University</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>IAU-019985-1</t>
+          <t>IAU-003340-1</t>
         </is>
       </c>
       <c r="C28" t="b">
@@ -1106,28 +1192,31 @@
         <v>1</v>
       </c>
       <c r="E28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28">
-        <v>2822</v>
+        <v>970</v>
+      </c>
+      <c r="H28">
+        <v>2015</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>(UCW)</t>
+          <t>Dalhousie University</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>IAU-019970-1</t>
+          <t>IAU-003505-3</t>
         </is>
       </c>
       <c r="C29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -1138,19 +1227,19 @@
       <c r="F29" t="b">
         <v>1</v>
       </c>
-      <c r="G29">
-        <v>2364</v>
+      <c r="H29">
+        <v>2015</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>(UFV)</t>
+          <t>Emily Carr University Of Art And Design</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>IAU-020555-1</t>
+          <t>IAU-004480-1</t>
         </is>
       </c>
       <c r="C30" t="b">
@@ -1166,157 +1255,175 @@
         <v>0</v>
       </c>
       <c r="G30">
-        <v>10935</v>
+        <v>1767</v>
+      </c>
+      <c r="H30">
+        <v>2015</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>(UM)</t>
+          <t>Fanshawe College</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>IAU-020275-1</t>
+          <t>IAU-006253-1</t>
         </is>
       </c>
       <c r="C31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" t="b">
         <v>1</v>
       </c>
       <c r="E31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
       </c>
       <c r="G31">
-        <v>30683</v>
+        <v>18080</v>
+      </c>
+      <c r="H31">
+        <v>2015</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>(UNB)</t>
+          <t>George Brown College</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>IAU-020328-1</t>
+          <t>IAU-006615-1</t>
         </is>
       </c>
       <c r="C32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
       </c>
       <c r="G32">
-        <v>9865</v>
+        <v>65696</v>
+      </c>
+      <c r="H32">
+        <v>2015</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>(UNBC)</t>
+          <t>Georgian College</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>IAU-020354-1</t>
+          <t>IAU-006626-1</t>
         </is>
       </c>
       <c r="C33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="b">
         <v>1</v>
       </c>
       <c r="E33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
       </c>
       <c r="G33">
-        <v>3603</v>
+        <v>11433</v>
+      </c>
+      <c r="H33">
+        <v>2015</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>(UOIT)</t>
+          <t>Grant Macewan University</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>IAU-020365-1</t>
+          <t>IAU-006768-1</t>
         </is>
       </c>
       <c r="C34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" t="b">
         <v>1</v>
       </c>
       <c r="E34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
       </c>
       <c r="G34">
-        <v>10000</v>
+        <v>14465</v>
+      </c>
+      <c r="H34">
+        <v>2015</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>(UPEI)</t>
+          <t>Humber College</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>IAU-020437-1</t>
+          <t>IAU-007625-1</t>
         </is>
       </c>
       <c r="C35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" t="b">
         <v>1</v>
       </c>
       <c r="E35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
       </c>
       <c r="G35">
-        <v>4573</v>
+        <v>20600</v>
+      </c>
+      <c r="H35">
+        <v>2015</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>(USMC)</t>
+          <t>Institute Of Theological Training Of Montreal</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>IAU-020599-020519-1</t>
+          <t>IAU-007925-1</t>
         </is>
       </c>
       <c r="C36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" t="b">
         <v>1</v>
@@ -1325,75 +1432,78 @@
         <v>1</v>
       </c>
       <c r="F36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36">
-        <v>64218</v>
+        <v>1545</v>
+      </c>
+      <c r="H36">
+        <v>2015</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>(UVic)</t>
+          <t>National Institute Of Scientific Research (University Of Quebec)</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>IAU-020613-1</t>
+          <t>IAU-008067-1</t>
         </is>
       </c>
       <c r="C37" t="b">
         <v>1</v>
       </c>
-      <c r="D37" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" t="b">
-        <v>1</v>
-      </c>
       <c r="F37" t="b">
         <v>0</v>
       </c>
       <c r="G37">
-        <v>21354</v>
+        <v>741</v>
+      </c>
+      <c r="H37">
+        <v>2015</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>(UW)</t>
+          <t>Institute For Christian Studies</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>IAU-020623-1</t>
+          <t>IAU-008327-1</t>
         </is>
       </c>
       <c r="C38" t="b">
         <v>1</v>
       </c>
       <c r="D38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" t="b">
         <v>1</v>
       </c>
       <c r="F38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38">
-        <v>39195</v>
+        <v>1995</v>
+      </c>
+      <c r="H38">
+        <v>2015</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>(UWINNIPEG)</t>
+          <t>Justice Institute Of British Columbia</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>IAU-016620-1</t>
+          <t>IAU-010009-1</t>
         </is>
       </c>
       <c r="C39" t="b">
@@ -1403,78 +1513,87 @@
         <v>1</v>
       </c>
       <c r="E39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
       </c>
       <c r="G39">
-        <v>10675</v>
+        <v>28285</v>
+      </c>
+      <c r="H39">
+        <v>2015</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Acadia university</t>
+          <t>Kwantlen Polytechnic University</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>IAU-000076-1</t>
+          <t>IAU-010661-1</t>
         </is>
       </c>
       <c r="C40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" t="b">
         <v>1</v>
       </c>
       <c r="E40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
       </c>
       <c r="G40">
-        <v>4349</v>
+        <v>15119</v>
+      </c>
+      <c r="H40">
+        <v>2015</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Acsenda School of Management - Vancouver</t>
+          <t>Lakehead University</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>IAU-022957-1</t>
+          <t>IAU-010811-1</t>
         </is>
       </c>
       <c r="C41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" t="b">
         <v>1</v>
       </c>
       <c r="E41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41">
-        <v>1845</v>
+        <v>7606</v>
+      </c>
+      <c r="H41">
+        <v>2015</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Algonquin College</t>
+          <t>Lakeland College</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>IAU-000830-1</t>
+          <t>IAU-010814-1</t>
         </is>
       </c>
       <c r="C42" t="b">
@@ -1490,18 +1609,22 @@
         <v>0</v>
       </c>
       <c r="G42">
-        <v>22348</v>
+        <v>2535</v>
+      </c>
+      <c r="H42">
+        <v>2015</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Ambrose University</t>
+          <t>Laurentian University
+Huntington University</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>IAU-000890-1</t>
+          <t>IAU-010871-007656-1</t>
         </is>
       </c>
       <c r="C43" t="b">
@@ -1514,21 +1637,24 @@
         <v>1</v>
       </c>
       <c r="F43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43">
-        <v>1014</v>
+        <v>2615</v>
+      </c>
+      <c r="H43">
+        <v>2015</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Athabasca University</t>
+          <t>Laurentian University</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>IAU-001258-1</t>
+          <t>IAU-010871-2</t>
         </is>
       </c>
       <c r="C44" t="b">
@@ -1543,19 +1669,19 @@
       <c r="F44" t="b">
         <v>0</v>
       </c>
-      <c r="G44">
-        <v>40541</v>
+      <c r="H44">
+        <v>2015</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Bishop's University</t>
+          <t>Lethbridge College</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>IAU-001686-1</t>
+          <t>IAU-010917-1</t>
         </is>
       </c>
       <c r="C45" t="b">
@@ -1565,51 +1691,57 @@
         <v>1</v>
       </c>
       <c r="E45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" t="b">
         <v>0</v>
       </c>
       <c r="G45">
-        <v>2835</v>
+        <v>4532</v>
+      </c>
+      <c r="H45">
+        <v>2015</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Booth University College</t>
+          <t>Mcgill University</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>IAU-001724-1</t>
+          <t>IAU-011496-1</t>
         </is>
       </c>
       <c r="C46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" t="b">
         <v>1</v>
       </c>
       <c r="E46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46">
-        <v>282</v>
+        <v>35356</v>
+      </c>
+      <c r="H46">
+        <v>2015</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Brescia University College</t>
+          <t>Mcmaster University</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>IAU-001755-1</t>
+          <t>IAU-011499-1</t>
         </is>
       </c>
       <c r="C47" t="b">
@@ -1622,21 +1754,24 @@
         <v>1</v>
       </c>
       <c r="F47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47">
-        <v>1518</v>
+        <v>28631</v>
+      </c>
+      <c r="H47">
+        <v>2015</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Briercrest College and Seminary</t>
+          <t>Medicine Hat College.</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>IAU-020476-023022-1</t>
+          <t>IAU-011516-1</t>
         </is>
       </c>
       <c r="C48" t="b">
@@ -1646,24 +1781,27 @@
         <v>1</v>
       </c>
       <c r="E48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48">
-        <v>2224</v>
+        <v>2428</v>
+      </c>
+      <c r="H48">
+        <v>2015</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Brock University</t>
+          <t>Memorial University Of Newfoundland</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>IAU-001778-1</t>
+          <t>IAU-011558-1</t>
         </is>
       </c>
       <c r="C49" t="b">
@@ -1679,18 +1817,21 @@
         <v>0</v>
       </c>
       <c r="G49">
-        <v>19029</v>
+        <v>18694</v>
+      </c>
+      <c r="H49">
+        <v>2015</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Burman University</t>
+          <t>Mount Allison University</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>IAU-001956-1</t>
+          <t>IAU-012185-1</t>
         </is>
       </c>
       <c r="C50" t="b">
@@ -1700,24 +1841,27 @@
         <v>1</v>
       </c>
       <c r="E50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" t="b">
         <v>1</v>
       </c>
       <c r="G50">
-        <v>479</v>
+        <v>2303</v>
+      </c>
+      <c r="H50">
+        <v>2015</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Camosun College</t>
+          <t>Mount Royal University</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>IAU-001940-1</t>
+          <t>IAU-012199-1</t>
         </is>
       </c>
       <c r="C51" t="b">
@@ -1733,22 +1877,25 @@
         <v>0</v>
       </c>
       <c r="G51">
-        <v>9793</v>
+        <v>12855</v>
+      </c>
+      <c r="H51">
+        <v>2015</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Cape Breton University</t>
+          <t>Mount Saint Vincent University</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>IAU-001969-1</t>
+          <t>IAU-012203-1</t>
         </is>
       </c>
       <c r="C52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52" t="b">
         <v>1</v>
@@ -1760,18 +1907,21 @@
         <v>0</v>
       </c>
       <c r="G52">
-        <v>3989</v>
+        <v>4075</v>
+      </c>
+      <c r="H52">
+        <v>2015</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Capilano University</t>
+          <t>Niagara College</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>IAU-001973-1</t>
+          <t>IAU-012666-1</t>
         </is>
       </c>
       <c r="C53" t="b">
@@ -1787,18 +1937,21 @@
         <v>0</v>
       </c>
       <c r="G53">
-        <v>6523</v>
+        <v>20026</v>
+      </c>
+      <c r="H53">
+        <v>2015</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Carleton University</t>
+          <t>Nipissing University</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>IAU-001997-1</t>
+          <t>IAU-012719-1</t>
         </is>
       </c>
       <c r="C54" t="b">
@@ -1814,18 +1967,21 @@
         <v>0</v>
       </c>
       <c r="G54">
-        <v>30889</v>
+        <v>4894</v>
+      </c>
+      <c r="H54">
+        <v>2015</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Centennial College</t>
+          <t>North Island College</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>IAU-002055-1</t>
+          <t>IAU-012786-1</t>
         </is>
       </c>
       <c r="C55" t="b">
@@ -1841,49 +1997,55 @@
         <v>0</v>
       </c>
       <c r="G55">
-        <v>26000</v>
+        <v>5553</v>
+      </c>
+      <c r="H55">
+        <v>2015</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Collège universitaire dominicain</t>
+          <t>Northern Alberta Institute Of Technology</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>IAU-003047-1</t>
+          <t>IAU-012815-1</t>
         </is>
       </c>
       <c r="C56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56" t="b">
         <v>1</v>
       </c>
       <c r="E56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G56">
-        <v>290</v>
+        <v>19507</v>
+      </c>
+      <c r="H56">
+        <v>2015</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Concordia University</t>
+          <t>Nscad University</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>IAU-003125-1</t>
+          <t>IAU-012923-1</t>
         </is>
       </c>
       <c r="C57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D57" t="b">
         <v>1</v>
@@ -1895,18 +2057,21 @@
         <v>0</v>
       </c>
       <c r="G57">
-        <v>46199</v>
+        <v>905</v>
+      </c>
+      <c r="H57">
+        <v>2015</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Concordia University of Edmonton</t>
+          <t>Okanagan College</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>IAU-003129-1</t>
+          <t>IAU-013031-1</t>
         </is>
       </c>
       <c r="C58" t="b">
@@ -1916,51 +2081,51 @@
         <v>1</v>
       </c>
       <c r="E58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G58">
-        <v>2234</v>
+        <v>7816</v>
+      </c>
+      <c r="H58">
+        <v>2015</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Conestoga College</t>
+          <t>Olds College</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>IAU-003135-1</t>
+          <t>IAU-013054-1</t>
         </is>
       </c>
       <c r="C59" t="b">
         <v>0</v>
       </c>
-      <c r="D59" t="b">
-        <v>1</v>
-      </c>
-      <c r="E59" t="b">
-        <v>0</v>
-      </c>
       <c r="F59" t="b">
         <v>0</v>
       </c>
       <c r="G59">
-        <v>12938</v>
+        <v>3342</v>
+      </c>
+      <c r="H59">
+        <v>2015</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Crandall University</t>
+          <t>Ocad University</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>IAU-003340-1</t>
+          <t>IAU-013094-1</t>
         </is>
       </c>
       <c r="C60" t="b">
@@ -1973,21 +2138,24 @@
         <v>1</v>
       </c>
       <c r="F60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G60">
-        <v>1104</v>
+        <v>4793</v>
+      </c>
+      <c r="H60">
+        <v>2015</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Dalhousie University</t>
+          <t>Providence University College And Theological Seminary</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>IAU-003505-3</t>
+          <t>IAU-013766-1</t>
         </is>
       </c>
       <c r="C61" t="b">
@@ -2001,71 +2169,77 @@
       </c>
       <c r="F61" t="b">
         <v>1</v>
+      </c>
+      <c r="G61">
+        <v>285</v>
+      </c>
+      <c r="H61">
+        <v>2015</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Ecole de Technologie supérieure (ETS)</t>
+          <t>Queen'S University</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>IAU-019700-004020-1</t>
+          <t>IAU-013841-1</t>
         </is>
       </c>
       <c r="C62" t="b">
-        <v>1</v>
-      </c>
-      <c r="D62" t="b">
-        <v>1</v>
-      </c>
-      <c r="E62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F62" t="b">
         <v>0</v>
       </c>
       <c r="G62">
-        <v>8970</v>
+        <v>23295</v>
+      </c>
+      <c r="H62">
+        <v>2015</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Ecole nationale d'Administration publique (ENAP)</t>
+          <t>Quest University Canada</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>IAU-019700-004084-1</t>
+          <t>IAU-013849-1</t>
         </is>
       </c>
       <c r="C63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G63">
-        <v>6507</v>
+        <v>420</v>
+      </c>
+      <c r="H63">
+        <v>2015</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Emily Carr University of Art and Design</t>
+          <t>Red Deer College</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>IAU-004480-1</t>
+          <t>IAU-013935-1</t>
         </is>
       </c>
       <c r="C64" t="b">
@@ -2075,24 +2249,27 @@
         <v>1</v>
       </c>
       <c r="E64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F64" t="b">
         <v>0</v>
       </c>
       <c r="G64">
-        <v>2006</v>
+        <v>7500</v>
+      </c>
+      <c r="H64">
+        <v>2015</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Fanshawe College</t>
+          <t>Redeemer University College</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>IAU-006253-1</t>
+          <t>IAU-013938-1</t>
         </is>
       </c>
       <c r="C65" t="b">
@@ -2105,75 +2282,84 @@
         <v>0</v>
       </c>
       <c r="F65" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G65">
-        <v>20270</v>
+        <v>939</v>
+      </c>
+      <c r="H65">
+        <v>2015</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Georgian College</t>
+          <t>Royal Military College Of Canada</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>IAU-006626-1</t>
+          <t>IAU-014124-1</t>
         </is>
       </c>
       <c r="C66" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D66" t="b">
         <v>1</v>
       </c>
       <c r="E66" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F66" t="b">
         <v>0</v>
       </c>
       <c r="G66">
-        <v>13000</v>
+        <v>1797</v>
+      </c>
+      <c r="H66">
+        <v>2015</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Grant MacEwan University</t>
+          <t>Royal Roads University</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>IAU-006768-1</t>
+          <t>IAU-014126-1</t>
         </is>
       </c>
       <c r="C67" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67" t="b">
         <v>1</v>
       </c>
       <c r="E67" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F67" t="b">
         <v>0</v>
       </c>
       <c r="G67">
-        <v>17103</v>
+        <v>3353</v>
+      </c>
+      <c r="H67">
+        <v>2015</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>HEC Montréal (HEC)</t>
+          <t>Ryerson University</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>IAU-019623-007137-1</t>
+          <t>IAU-014158-1</t>
         </is>
       </c>
       <c r="C68" t="b">
@@ -2189,45 +2375,51 @@
         <v>0</v>
       </c>
       <c r="G68">
-        <v>61864</v>
+        <v>33328</v>
+      </c>
+      <c r="H68">
+        <v>2015</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Humber College</t>
+          <t>Saint Mary'S University</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>IAU-007625-1</t>
+          <t>IAU-014271-1</t>
         </is>
       </c>
       <c r="C69" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69" t="b">
         <v>1</v>
       </c>
       <c r="E69" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F69" t="b">
         <v>0</v>
       </c>
       <c r="G69">
-        <v>25400</v>
+        <v>7728</v>
+      </c>
+      <c r="H69">
+        <v>2015</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Institut de Formation Théologique de Montréal (IFTM)</t>
+          <t>Seneca College.</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>IAU-007925-1</t>
+          <t>IAU-015159-1</t>
         </is>
       </c>
       <c r="C70" t="b">
@@ -2237,72 +2429,87 @@
         <v>1</v>
       </c>
       <c r="E70" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F70" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G70">
-        <v>1586</v>
+        <v>26384</v>
+      </c>
+      <c r="H70">
+        <v>2015</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Institut national de la Recherche scientifique (Université du Québec) (INRS)</t>
+          <t>Sheridan College Institute Of Technology And Advanced Learning</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>IAU-008067-1</t>
+          <t>IAU-015318-1</t>
         </is>
       </c>
       <c r="C71" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D71" t="b">
+        <v>1</v>
+      </c>
+      <c r="E71" t="b">
+        <v>0</v>
       </c>
       <c r="F71" t="b">
         <v>0</v>
       </c>
       <c r="G71">
-        <v>844</v>
+        <v>16840</v>
+      </c>
+      <c r="H71">
+        <v>2015</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Institute for Christian Studies</t>
+          <t>Simon Fraser University</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>IAU-008327-1</t>
+          <t>IAU-015440-1</t>
         </is>
       </c>
       <c r="C72" t="b">
         <v>1</v>
       </c>
       <c r="D72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E72" t="b">
         <v>1</v>
       </c>
       <c r="F72" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G72">
-        <v>2481</v>
+        <v>29673</v>
+      </c>
+      <c r="H72">
+        <v>2015</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Justice Institute of British Columbia</t>
+          <t>Southern Alberta Institute Of Technology</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>IAU-010009-1</t>
+          <t>IAU-015594-1</t>
         </is>
       </c>
       <c r="C73" t="b">
@@ -2318,18 +2525,21 @@
         <v>0</v>
       </c>
       <c r="G73">
-        <v>29428</v>
+        <v>12633</v>
+      </c>
+      <c r="H73">
+        <v>2015</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Kingswood University</t>
+          <t>St. Francis Xavier University</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>IAU-001620-1</t>
+          <t>IAU-015743-1</t>
         </is>
       </c>
       <c r="C74" t="b">
@@ -2342,21 +2552,24 @@
         <v>1</v>
       </c>
       <c r="F74" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G74">
-        <v>352</v>
+        <v>4432</v>
+      </c>
+      <c r="H74">
+        <v>2015</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Kwantlen Polytechnic University</t>
+          <t>St. Jerome'S University (University Of Waterloo)</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>IAU-010661-1</t>
+          <t>IAU-015746-1</t>
         </is>
       </c>
       <c r="C75" t="b">
@@ -2366,24 +2579,27 @@
         <v>1</v>
       </c>
       <c r="E75" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F75" t="b">
         <v>0</v>
       </c>
       <c r="G75">
-        <v>14008</v>
+        <v>896</v>
+      </c>
+      <c r="H75">
+        <v>2015</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>La Cité</t>
+          <t>St. Lawrence College</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>IAU-002993-1</t>
+          <t>IAU-015759-1</t>
         </is>
       </c>
       <c r="C76" t="b">
@@ -2396,48 +2612,54 @@
         <v>0</v>
       </c>
       <c r="F76" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G76">
-        <v>3710</v>
+        <v>5892</v>
+      </c>
+      <c r="H76">
+        <v>2015</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Lakehead university</t>
+          <t>St. Mary'S University</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>IAU-010811-1</t>
+          <t>IAU-015769-1</t>
         </is>
       </c>
       <c r="C77" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D77" t="b">
         <v>1</v>
       </c>
       <c r="E77" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F77" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G77">
-        <v>8162</v>
+        <v>527</v>
+      </c>
+      <c r="H77">
+        <v>2015</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Lakeland College</t>
+          <t>St. Stephen'S University</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>IAU-010814-1</t>
+          <t>IAU-015791-1</t>
         </is>
       </c>
       <c r="C78" t="b">
@@ -2447,24 +2669,27 @@
         <v>1</v>
       </c>
       <c r="E78" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G78">
-        <v>5571</v>
+        <v>114</v>
+      </c>
+      <c r="H78">
+        <v>2015</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Laurentian University/Université Laurentienne</t>
+          <t>The King'S University</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>IAU-010871-007656-1</t>
+          <t>IAU-016483-1</t>
         </is>
       </c>
       <c r="C79" t="b">
@@ -2474,24 +2699,27 @@
         <v>1</v>
       </c>
       <c r="E79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F79" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G79">
-        <v>3075</v>
+        <v>789</v>
+      </c>
+      <c r="H79">
+        <v>2015</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Laval University</t>
+          <t>The University Of British Columbia</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>IAU-019754-1</t>
+          <t>IAU-016562-1</t>
         </is>
       </c>
       <c r="C80" t="b">
@@ -2507,18 +2735,21 @@
         <v>0</v>
       </c>
       <c r="G80">
-        <v>42049</v>
+        <v>55734</v>
+      </c>
+      <c r="H80">
+        <v>2015</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Lethbridge College</t>
+          <t>The University Of Winnipeg</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>IAU-010917-1</t>
+          <t>IAU-016620-1</t>
         </is>
       </c>
       <c r="C81" t="b">
@@ -2528,28 +2759,31 @@
         <v>1</v>
       </c>
       <c r="E81" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F81" t="b">
         <v>0</v>
       </c>
       <c r="G81">
-        <v>5154</v>
+        <v>9519</v>
+      </c>
+      <c r="H81">
+        <v>2015</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Mcgill University</t>
+          <t>Thompson Rivers University</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>IAU-011496-1</t>
+          <t>IAU-016643-1</t>
         </is>
       </c>
       <c r="C82" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D82" t="b">
         <v>1</v>
@@ -2561,22 +2795,25 @@
         <v>0</v>
       </c>
       <c r="G82">
-        <v>38133</v>
+        <v>9715</v>
+      </c>
+      <c r="H82">
+        <v>2015</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>McMaster university</t>
+          <t>Trent University</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>IAU-011499-1</t>
+          <t>IAU-016840-1</t>
         </is>
       </c>
       <c r="C83" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D83" t="b">
         <v>1</v>
@@ -2585,25 +2822,28 @@
         <v>1</v>
       </c>
       <c r="F83" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G83">
-        <v>31843</v>
+        <v>9397</v>
+      </c>
+      <c r="H83">
+        <v>2015</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Memorial University of Newfoundland (Memorial University College)</t>
+          <t>Trinity Western University</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>IAU-011558-1</t>
+          <t>IAU-016857-1</t>
         </is>
       </c>
       <c r="C84" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D84" t="b">
         <v>1</v>
@@ -2612,25 +2852,28 @@
         <v>1</v>
       </c>
       <c r="F84" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G84">
-        <v>19233</v>
+        <v>3970</v>
+      </c>
+      <c r="H84">
+        <v>2015</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Mount Allison university</t>
+          <t>Tyndale University College And Seminary</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>IAU-012185-1</t>
+          <t>IAU-016965-1</t>
         </is>
       </c>
       <c r="C85" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D85" t="b">
         <v>1</v>
@@ -2642,45 +2885,52 @@
         <v>1</v>
       </c>
       <c r="G85">
-        <v>2357</v>
+        <v>1196</v>
+      </c>
+      <c r="H85">
+        <v>2015</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Mount Royal University</t>
+          <t>University Of Moncton</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>IAU-012199-1</t>
+          <t>IAU-019621-1</t>
         </is>
       </c>
       <c r="C86" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D86" t="b">
         <v>1</v>
       </c>
       <c r="E86" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F86" t="b">
         <v>0</v>
       </c>
       <c r="G86">
-        <v>14233</v>
+        <v>5812</v>
+      </c>
+      <c r="H86">
+        <v>2015</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Mount Saint Vincent University (formerly a college)</t>
+          <t>University Of Montreal
+Polytechnic School Of Montreal</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>IAU-012203-1</t>
+          <t>IAU-019623-004208-1</t>
         </is>
       </c>
       <c r="C87" t="b">
@@ -2696,45 +2946,52 @@
         <v>0</v>
       </c>
       <c r="G87">
-        <v>4312</v>
+        <v>12120</v>
+      </c>
+      <c r="H87">
+        <v>2015</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Niagara College of Applied Arts and Technology</t>
+          <t>University Of Montreal
+Hec Montreal</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>IAU-012666-1</t>
+          <t>IAU-019623-007137-1</t>
         </is>
       </c>
       <c r="C88" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D88" t="b">
         <v>1</v>
       </c>
       <c r="E88" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F88" t="b">
         <v>0</v>
       </c>
       <c r="G88">
-        <v>22770</v>
+        <v>47447</v>
+      </c>
+      <c r="H88">
+        <v>2015</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Nipissing University</t>
+          <t>University Of Montreal</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>IAU-012719-1</t>
+          <t>IAU-019623-1</t>
         </is>
       </c>
       <c r="C89" t="b">
@@ -2750,49 +3007,56 @@
         <v>0</v>
       </c>
       <c r="G89">
-        <v>5259</v>
+        <v>57696</v>
+      </c>
+      <c r="H89">
+        <v>2015</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>North Island College</t>
+          <t>University Of Sherbrooke</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>IAU-012786-1</t>
+          <t>IAU-019648-1</t>
         </is>
       </c>
       <c r="C90" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D90" t="b">
         <v>1</v>
       </c>
       <c r="E90" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F90" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G90">
-        <v>6314</v>
+        <v>37144</v>
+      </c>
+      <c r="H90">
+        <v>2015</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Nova Scotia College of Art and Design (NSCAD)</t>
+          <t>University Of Quebec
+Engineering School - Ets</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>IAU-012923-1</t>
+          <t>IAU-019700-004020-1</t>
         </is>
       </c>
       <c r="C91" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D91" t="b">
         <v>1</v>
@@ -2804,45 +3068,52 @@
         <v>0</v>
       </c>
       <c r="G91">
-        <v>710</v>
+        <v>7708</v>
+      </c>
+      <c r="H91">
+        <v>2015</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Pacific Coast University for Workplace Health Sciences</t>
+          <t>University Of Quebec
+National School Of Public Administration</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>IAU-022840-1</t>
+          <t>IAU-019700-004084-1</t>
         </is>
       </c>
       <c r="C92" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D92" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E92" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F92" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G92">
-        <v>1865</v>
+        <v>5532</v>
+      </c>
+      <c r="H92">
+        <v>2015</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Polytechnique Montréal</t>
+          <t>University Of Quebec</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>IAU-019623-004208-1</t>
+          <t>IAU-019700-1</t>
         </is>
       </c>
       <c r="C93" t="b">
@@ -2858,207 +3129,189 @@
         <v>0</v>
       </c>
       <c r="G93">
-        <v>50308</v>
+        <v>90540</v>
+      </c>
+      <c r="H93">
+        <v>2015</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Providence University College and Theological Seminary</t>
+          <t>University Of Quebec At Chicoutimi</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>IAU-013766-1</t>
+          <t>IAU-019701-1</t>
         </is>
       </c>
       <c r="C94" t="b">
         <v>1</v>
       </c>
-      <c r="D94" t="b">
-        <v>1</v>
-      </c>
-      <c r="E94" t="b">
-        <v>1</v>
-      </c>
       <c r="F94" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G94">
-        <v>325</v>
+        <v>351</v>
+      </c>
+      <c r="H94">
+        <v>2015</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Queen's University (at Kingston)</t>
+          <t>Tele-University</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>IAU-013841-1</t>
+          <t>IAU-019702-1</t>
         </is>
       </c>
       <c r="C95" t="b">
         <v>1</v>
       </c>
-      <c r="D95" t="b">
-        <v>1</v>
-      </c>
-      <c r="E95" t="b">
-        <v>1</v>
-      </c>
       <c r="F95" t="b">
         <v>0</v>
       </c>
       <c r="G95">
-        <v>29923</v>
+        <v>15455</v>
+      </c>
+      <c r="H95">
+        <v>2015</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Quest University Canada</t>
+          <t>University Of Quebec At Montreal</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>IAU-013849-1</t>
+          <t>IAU-019703-1</t>
         </is>
       </c>
       <c r="C96" t="b">
         <v>0</v>
       </c>
-      <c r="D96" t="b">
-        <v>1</v>
-      </c>
-      <c r="E96" t="b">
-        <v>0</v>
-      </c>
       <c r="F96" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G96">
-        <v>494</v>
+        <v>47029</v>
+      </c>
+      <c r="H96">
+        <v>2015</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Redeemer University College</t>
+          <t>University Of Quebec At Rimouski</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>IAU-013938-1</t>
+          <t>IAU-019704-1</t>
         </is>
       </c>
       <c r="C97" t="b">
-        <v>0</v>
-      </c>
-      <c r="D97" t="b">
-        <v>1</v>
-      </c>
-      <c r="E97" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F97" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G97">
-        <v>1139</v>
+        <v>7128</v>
+      </c>
+      <c r="H97">
+        <v>2015</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Royal Military College of Canada</t>
+          <t>University Of Quebec At Trois-RivièRes</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>IAU-014124-1</t>
+          <t>IAU-019705-1</t>
         </is>
       </c>
       <c r="C98" t="b">
         <v>1</v>
       </c>
-      <c r="D98" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" t="b">
-        <v>1</v>
-      </c>
       <c r="F98" t="b">
         <v>0</v>
       </c>
       <c r="G98">
-        <v>2263</v>
+        <v>13333</v>
+      </c>
+      <c r="H98">
+        <v>2015</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Royal Roads University (Royal Roads Military College)</t>
+          <t>University Of Quebec Abitibi-Temiscamingue</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>IAU-014126-1</t>
+          <t>IAU-019706-1</t>
         </is>
       </c>
       <c r="C99" t="b">
         <v>1</v>
       </c>
-      <c r="D99" t="b">
-        <v>1</v>
-      </c>
-      <c r="E99" t="b">
-        <v>1</v>
-      </c>
       <c r="F99" t="b">
         <v>0</v>
       </c>
       <c r="G99">
-        <v>3937</v>
+        <v>4118</v>
+      </c>
+      <c r="H99">
+        <v>2015</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Ryerson University (Ryerson Polytechnical Institute)</t>
+          <t>University Of Quebec In Outaouais</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>IAU-014158-1</t>
+          <t>IAU-019707-1</t>
         </is>
       </c>
       <c r="C100" t="b">
         <v>1</v>
       </c>
-      <c r="D100" t="b">
-        <v>1</v>
-      </c>
-      <c r="E100" t="b">
-        <v>1</v>
-      </c>
       <c r="F100" t="b">
         <v>0</v>
       </c>
       <c r="G100">
-        <v>44950</v>
+        <v>6311</v>
+      </c>
+      <c r="H100">
+        <v>2015</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Saint Mary's University</t>
+          <t>Laval University</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>IAU-014271-1</t>
+          <t>IAU-019754-1</t>
         </is>
       </c>
       <c r="C101" t="b">
@@ -3074,22 +3327,25 @@
         <v>0</v>
       </c>
       <c r="G101">
-        <v>8091</v>
+        <v>39672</v>
+      </c>
+      <c r="H101">
+        <v>2015</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Saint Paul University / Université Saint Paul</t>
+          <t>Saint-Anne University</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>IAU-020369-020368-1</t>
+          <t>IAU-019836-1</t>
         </is>
       </c>
       <c r="C102" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D102" t="b">
         <v>1</v>
@@ -3101,18 +3357,21 @@
         <v>0</v>
       </c>
       <c r="G102">
-        <v>37184</v>
+        <v>2091</v>
+      </c>
+      <c r="H102">
+        <v>2015</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>SAIT Polytechnic (SAIT)</t>
+          <t>University Canada West</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>IAU-015594-1</t>
+          <t>IAU-019970-1</t>
         </is>
       </c>
       <c r="C103" t="b">
@@ -3122,24 +3381,27 @@
         <v>1</v>
       </c>
       <c r="E103" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F103" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G103">
-        <v>14364</v>
+        <v>2175</v>
+      </c>
+      <c r="H103">
+        <v>2015</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Seneca College</t>
+          <t>University College Of The North</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>IAU-015159-1</t>
+          <t>IAU-019985-1</t>
         </is>
       </c>
       <c r="C104" t="b">
@@ -3155,45 +3417,48 @@
         <v>0</v>
       </c>
       <c r="G104">
-        <v>30000</v>
+        <v>2400</v>
+      </c>
+      <c r="H104">
+        <v>2015</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Sheridan College Institute of Technology and Advanced Learning</t>
+          <t>University Of Alberta</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>IAU-015318-1</t>
+          <t>IAU-020010-1</t>
         </is>
       </c>
       <c r="C105" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D105" t="b">
         <v>1</v>
       </c>
       <c r="E105" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F105" t="b">
         <v>0</v>
       </c>
-      <c r="G105">
-        <v>21600</v>
+      <c r="H105">
+        <v>2015</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Simon Fraser University</t>
+          <t>University Of Calgary</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>IAU-015440-1</t>
+          <t>IAU-020053-1</t>
         </is>
       </c>
       <c r="C106" t="b">
@@ -3209,22 +3474,25 @@
         <v>0</v>
       </c>
       <c r="G106">
-        <v>30300</v>
+        <v>29214</v>
+      </c>
+      <c r="H106">
+        <v>2015</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>St Francis Xavier University</t>
+          <t>University Of Guelph</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>IAU-015743-1</t>
+          <t>IAU-020173-1</t>
         </is>
       </c>
       <c r="C107" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D107" t="b">
         <v>1</v>
@@ -3233,75 +3501,79 @@
         <v>1</v>
       </c>
       <c r="F107" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G107">
-        <v>4048</v>
+        <v>24699</v>
+      </c>
+      <c r="H107">
+        <v>2015</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>St. John's College (University of Manitoba)</t>
+          <t>University Of King’S College</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>IAU-020275-015752-1</t>
+          <t>IAU-020215-1</t>
         </is>
       </c>
       <c r="C108" t="b">
-        <v>1</v>
-      </c>
-      <c r="D108" t="b">
-        <v>1</v>
-      </c>
-      <c r="E108" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F108" t="b">
         <v>0</v>
       </c>
       <c r="G108">
-        <v>31037</v>
+        <v>1134</v>
+      </c>
+      <c r="H108">
+        <v>2015</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>St. Mary's University</t>
+          <t>University Of Lethbridge</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>IAU-015769-1</t>
+          <t>IAU-020225-1</t>
         </is>
       </c>
       <c r="C109" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D109" t="b">
         <v>1</v>
       </c>
       <c r="E109" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F109" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G109">
-        <v>600</v>
+        <v>8205</v>
+      </c>
+      <c r="H109">
+        <v>2015</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>St. Paul's College (University of Manitoba)</t>
+          <t>University Of Manitoba
+St. John'S College (University Of Manitoba)</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>IAU-020275-015783-1</t>
+          <t>IAU-020275-015752-1</t>
         </is>
       </c>
       <c r="C110" t="b">
@@ -3317,66 +3589,82 @@
         <v>0</v>
       </c>
       <c r="G110">
-        <v>22512</v>
+        <v>27296</v>
+      </c>
+      <c r="H110">
+        <v>2015</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Tele-universite</t>
+          <t>University Of Manitoba
+St. Paul'S College (University Of Manitoba)</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>IAU-019702-1</t>
+          <t>IAU-020275-015783-1</t>
         </is>
       </c>
       <c r="C111" t="b">
         <v>1</v>
       </c>
+      <c r="D111" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" t="b">
+        <v>1</v>
+      </c>
       <c r="F111" t="b">
         <v>0</v>
       </c>
       <c r="G111">
-        <v>18701</v>
+        <v>3757</v>
+      </c>
+      <c r="H111">
+        <v>2015</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>The King's University</t>
+          <t>University Of Manitoba</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>IAU-016483-1</t>
+          <t>IAU-020275-1</t>
         </is>
       </c>
       <c r="C112" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D112" t="b">
         <v>1</v>
       </c>
       <c r="E112" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F112" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G112">
-        <v>875</v>
+        <v>29557</v>
+      </c>
+      <c r="H112">
+        <v>2015</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Trent University</t>
+          <t>University Of New Brunswick</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>IAU-016840-1</t>
+          <t>IAU-020328-1</t>
         </is>
       </c>
       <c r="C113" t="b">
@@ -3392,22 +3680,25 @@
         <v>0</v>
       </c>
       <c r="G113">
-        <v>10905</v>
+        <v>10372</v>
+      </c>
+      <c r="H113">
+        <v>2015</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Trinity Western University</t>
+          <t>University Of Northern British Columbia</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>IAU-016857-1</t>
+          <t>IAU-020354-1</t>
         </is>
       </c>
       <c r="C114" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D114" t="b">
         <v>1</v>
@@ -3416,21 +3707,24 @@
         <v>1</v>
       </c>
       <c r="F114" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G114">
-        <v>4000</v>
+        <v>3839</v>
+      </c>
+      <c r="H114">
+        <v>2015</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Tyndale University College and Seminary</t>
+          <t>University Of Ontario Institute Of Technology</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>IAU-016965-1</t>
+          <t>IAU-020365-1</t>
         </is>
       </c>
       <c r="C115" t="b">
@@ -3443,21 +3737,25 @@
         <v>1</v>
       </c>
       <c r="F115" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G115">
-        <v>1361</v>
+        <v>8794</v>
+      </c>
+      <c r="H115">
+        <v>2015</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Université de Moncton</t>
+          <t>University Of Ottawa
+Saint Paul University</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>IAU-019621-1</t>
+          <t>IAU-020369-020368-1</t>
         </is>
       </c>
       <c r="C116" t="b">
@@ -3473,18 +3771,21 @@
         <v>0</v>
       </c>
       <c r="G116">
-        <v>5373</v>
+        <v>25773</v>
+      </c>
+      <c r="H116">
+        <v>2015</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Université de Montréal (UdeM)</t>
+          <t>University Of Ottawa</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>IAU-019623-1</t>
+          <t>IAU-020369-1</t>
         </is>
       </c>
       <c r="C117" t="b">
@@ -3500,22 +3801,25 @@
         <v>0</v>
       </c>
       <c r="G117">
-        <v>64573</v>
+        <v>42003</v>
+      </c>
+      <c r="H117">
+        <v>2015</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Université de Saint-Boniface (CUSB)</t>
+          <t>University Of Prince Edward Island</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>IAU-003046-1</t>
+          <t>IAU-020437-1</t>
         </is>
       </c>
       <c r="C118" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D118" t="b">
         <v>1</v>
@@ -3527,18 +3831,21 @@
         <v>0</v>
       </c>
       <c r="G118">
-        <v>1322</v>
+        <v>4322</v>
+      </c>
+      <c r="H118">
+        <v>2015</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Université de Sherbrooke (UdeS)</t>
+          <t>University Of Regina</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>IAU-019648-1</t>
+          <t>IAU-020447-1</t>
         </is>
       </c>
       <c r="C119" t="b">
@@ -3551,25 +3858,29 @@
         <v>1</v>
       </c>
       <c r="F119" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G119">
-        <v>33571</v>
+        <v>13448</v>
+      </c>
+      <c r="H119">
+        <v>2015</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Université du Québec (UQ)</t>
+          <t>University Of Saskatchewan
+Briercrest College And Seminary</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>IAU-019700-1</t>
+          <t>IAU-020476-023022-1</t>
         </is>
       </c>
       <c r="C120" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D120" t="b">
         <v>1</v>
@@ -3578,147 +3889,208 @@
         <v>1</v>
       </c>
       <c r="F120" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G120">
-        <v>101358</v>
+        <v>2176</v>
+      </c>
+      <c r="H120">
+        <v>2015</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Université du Québec à Chicoutimi (UQAC)</t>
+          <t>University Of Saskatchewan</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>IAU-019701-1</t>
+          <t>IAU-020476-1</t>
         </is>
       </c>
       <c r="C121" t="b">
         <v>1</v>
       </c>
+      <c r="D121" t="b">
+        <v>1</v>
+      </c>
+      <c r="E121" t="b">
+        <v>1</v>
+      </c>
       <c r="F121" t="b">
         <v>0</v>
       </c>
       <c r="G121">
-        <v>400</v>
+        <v>21450</v>
+      </c>
+      <c r="H121">
+        <v>2015</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Université du Québec à Montréal (UQAM)</t>
+          <t>University Of The Fraser Valley</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>IAU-019703-1</t>
+          <t>IAU-020555-1</t>
         </is>
       </c>
       <c r="C122" t="b">
+        <v>0</v>
+      </c>
+      <c r="D122" t="b">
+        <v>1</v>
+      </c>
+      <c r="E122" t="b">
         <v>1</v>
       </c>
       <c r="F122" t="b">
         <v>0</v>
       </c>
       <c r="G122">
-        <v>53474</v>
+        <v>14534</v>
+      </c>
+      <c r="H122">
+        <v>2015</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Université du Québec à Rimouski (UQAR)</t>
+          <t>University Of Toronto
+University Of St. Michael'S College</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>IAU-019704-1</t>
+          <t>IAU-020599-020519-1</t>
         </is>
       </c>
       <c r="C123" t="b">
         <v>1</v>
       </c>
+      <c r="D123" t="b">
+        <v>1</v>
+      </c>
+      <c r="E123" t="b">
+        <v>1</v>
+      </c>
       <c r="F123" t="b">
         <v>0</v>
       </c>
       <c r="G123">
-        <v>6842</v>
+        <v>56479</v>
+      </c>
+      <c r="H123">
+        <v>2015</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Université du Québec à Trois-Rivières (UQTR)</t>
+          <t>University Of Toronto
+University Of Trinity College</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>IAU-019705-1</t>
+          <t>IAU-020599-020601-1</t>
         </is>
       </c>
       <c r="C124" t="b">
         <v>1</v>
       </c>
+      <c r="D124" t="b">
+        <v>1</v>
+      </c>
+      <c r="E124" t="b">
+        <v>1</v>
+      </c>
       <c r="F124" t="b">
         <v>0</v>
       </c>
       <c r="G124">
-        <v>14166</v>
+        <v>56479</v>
+      </c>
+      <c r="H124">
+        <v>2015</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Université du Québec en Abitibi-Témiscamingue (UQAT)</t>
+          <t>University Of Toronto
+Victoria University</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>IAU-019706-1</t>
+          <t>IAU-020599-020869-1</t>
         </is>
       </c>
       <c r="C125" t="b">
         <v>1</v>
       </c>
+      <c r="D125" t="b">
+        <v>1</v>
+      </c>
+      <c r="E125" t="b">
+        <v>1</v>
+      </c>
       <c r="F125" t="b">
         <v>0</v>
       </c>
       <c r="G125">
-        <v>4890</v>
+        <v>56479</v>
+      </c>
+      <c r="H125">
+        <v>2015</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Université du Québec en Outaouais (UQO)</t>
+          <t>University Of Toronto
+Wycliffe College</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>IAU-019707-1</t>
+          <t>IAU-020599-021367-1</t>
         </is>
       </c>
       <c r="C126" t="b">
         <v>1</v>
       </c>
+      <c r="D126" t="b">
+        <v>0</v>
+      </c>
+      <c r="E126" t="b">
+        <v>1</v>
+      </c>
       <c r="F126" t="b">
         <v>0</v>
       </c>
       <c r="G126">
-        <v>6115</v>
+        <v>56479</v>
+      </c>
+      <c r="H126">
+        <v>2015</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Université Laurentienne (LU)</t>
+          <t>University Of Toronto</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>IAU-010871-2</t>
+          <t>IAU-020599-1</t>
         </is>
       </c>
       <c r="C127" t="b">
@@ -3731,22 +4103,28 @@
         <v>1</v>
       </c>
       <c r="F127" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G127">
+        <v>78713</v>
+      </c>
+      <c r="H127">
+        <v>2015</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Université Sainte-Anne</t>
+          <t>University Of Victoria</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>IAU-019836-1</t>
+          <t>IAU-020613-1</t>
         </is>
       </c>
       <c r="C128" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D128" t="b">
         <v>1</v>
@@ -3758,22 +4136,25 @@
         <v>0</v>
       </c>
       <c r="G128">
-        <v>1244</v>
+        <v>20500</v>
+      </c>
+      <c r="H128">
+        <v>2015</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>University of King's College</t>
+          <t>University Of Waterloo</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>IAU-020215-1</t>
+          <t>IAU-020623-1</t>
         </is>
       </c>
       <c r="C129" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D129" t="b">
         <v>1</v>
@@ -3785,22 +4166,26 @@
         <v>0</v>
       </c>
       <c r="G129">
-        <v>983</v>
+        <v>34668</v>
+      </c>
+      <c r="H129">
+        <v>2015</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>University of Ottawa - Université d'Ottawa (uOttawa)</t>
+          <t>University Of Western Ontario
+Huron University College</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>IAU-020369-1</t>
+          <t>IAU-020629-007657-1</t>
         </is>
       </c>
       <c r="C130" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D130" t="b">
         <v>1</v>
@@ -3812,18 +4197,21 @@
         <v>0</v>
       </c>
       <c r="G130">
-        <v>41828</v>
+        <v>35386</v>
+      </c>
+      <c r="H130">
+        <v>2015</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>University of Trinity College</t>
+          <t>University Of Western Ontario</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>IAU-020599-020601-1</t>
+          <t>IAU-020629-1</t>
         </is>
       </c>
       <c r="C131" t="b">
@@ -3839,13 +4227,16 @@
         <v>0</v>
       </c>
       <c r="G131">
-        <v>64218</v>
+        <v>30716</v>
+      </c>
+      <c r="H131">
+        <v>2015</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>University of Windsor</t>
+          <t>University Of Windsor</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3866,7 +4257,10 @@
         <v>0</v>
       </c>
       <c r="G132">
-        <v>16321</v>
+        <v>16148</v>
+      </c>
+      <c r="H132">
+        <v>2015</v>
       </c>
     </row>
     <row r="133">
@@ -3893,18 +4287,21 @@
         <v>0</v>
       </c>
       <c r="G133">
-        <v>9764</v>
+        <v>15363</v>
+      </c>
+      <c r="H133">
+        <v>2015</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Victoria University</t>
+          <t>Wilfrid Laurier University</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>IAU-020599-020869-1</t>
+          <t>IAU-021264-1</t>
         </is>
       </c>
       <c r="C134" t="b">
@@ -3920,18 +4317,21 @@
         <v>0</v>
       </c>
       <c r="G134">
-        <v>64218</v>
+        <v>18588</v>
+      </c>
+      <c r="H134">
+        <v>2015</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Western University (UWO)</t>
+          <t>York University</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>IAU-020629-1</t>
+          <t>IAU-021739-1</t>
         </is>
       </c>
       <c r="C135" t="b">
@@ -3947,22 +4347,25 @@
         <v>0</v>
       </c>
       <c r="G135">
-        <v>36539</v>
+        <v>53146</v>
+      </c>
+      <c r="H135">
+        <v>2015</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Wilfrid Laurier University (waterloo lutheran university)</t>
+          <t>Yorkville University</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>IAU-021264-1</t>
+          <t>IAU-021740-1</t>
         </is>
       </c>
       <c r="C136" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D136" t="b">
         <v>1</v>
@@ -3971,75 +4374,84 @@
         <v>1</v>
       </c>
       <c r="F136" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G136">
-        <v>19822</v>
+        <v>2175</v>
+      </c>
+      <c r="H136">
+        <v>2015</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Wycliffe College</t>
+          <t>The Art Institute Of Vancouver</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>IAU-020599-021367-1</t>
+          <t>IAU-022835-1</t>
         </is>
       </c>
       <c r="C137" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D137" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E137" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F137" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G137">
-        <v>64218</v>
+        <v>1617</v>
+      </c>
+      <c r="H137">
+        <v>2015</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>York University</t>
+          <t>Pacific Coast University For Workplace Health Sciences</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>IAU-021739-1</t>
+          <t>IAU-022840-1</t>
         </is>
       </c>
       <c r="C138" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D138" t="b">
         <v>1</v>
       </c>
       <c r="E138" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F138" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G138">
-        <v>54928</v>
+        <v>1622</v>
+      </c>
+      <c r="H138">
+        <v>2015</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Yorkville University</t>
+          <t>Yukon College</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>IAU-021740-1</t>
+          <t>IAU-022843-1</t>
         </is>
       </c>
       <c r="C139" t="b">
@@ -4049,24 +4461,27 @@
         <v>1</v>
       </c>
       <c r="E139" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F139" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G139">
-        <v>2362</v>
+        <v>1909</v>
+      </c>
+      <c r="H139">
+        <v>2015</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Yukon College</t>
+          <t>Acsenda School Of Management - Vancouver</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>IAU-022843-1</t>
+          <t>IAU-022957-1</t>
         </is>
       </c>
       <c r="C140" t="b">
@@ -4079,10 +4494,13 @@
         <v>0</v>
       </c>
       <c r="F140" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G140">
-        <v>4656</v>
+        <v>1616</v>
+      </c>
+      <c r="H140">
+        <v>2015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
paper requests; modeling updates; pipeline rerun; gcp storage
</commit_message>
<xml_diff>
--- a/tasks/university_covariates/hand/canadian_universities.xlsx
+++ b/tasks/university_covariates/hand/canadian_universities.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H140"/>
+  <dimension ref="A1:I140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -366,35 +366,40 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>glued_id</t>
+          <t>uni_id</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>coordinates</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>phd_granting</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>bachelors_granting</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>masters_granting</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>private</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>enrollment_count</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>year</t>
         </is>
@@ -411,8 +416,10 @@
           <t>IAU-000076-1</t>
         </is>
       </c>
-      <c r="C2" t="b">
-        <v>1</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>45.0875592, -64.3662493</t>
+        </is>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -421,12 +428,15 @@
         <v>1</v>
       </c>
       <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>3869</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>2015</v>
       </c>
     </row>
@@ -441,22 +451,27 @@
           <t>IAU-000812-1</t>
         </is>
       </c>
-      <c r="C3" t="b">
-        <v>0</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>51.0619506, -114.0913314</t>
+        </is>
       </c>
       <c r="D3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
       </c>
       <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>1247</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>2015</v>
       </c>
     </row>
@@ -471,22 +486,27 @@
           <t>IAU-000830-1</t>
         </is>
       </c>
-      <c r="C4" t="b">
-        <v>0</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>45.3499278, -75.7549368</t>
+        </is>
       </c>
       <c r="D4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>19000</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>2015</v>
       </c>
     </row>
@@ -501,11 +521,13 @@
           <t>IAU-000890-1</t>
         </is>
       </c>
-      <c r="C5" t="b">
-        <v>0</v>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>51.0339643, -114.1934126</t>
+        </is>
       </c>
       <c r="D5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -513,10 +535,13 @@
       <c r="F5" t="b">
         <v>1</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5">
         <v>842</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>2015</v>
       </c>
     </row>
@@ -531,8 +556,10 @@
           <t>IAU-001258-1</t>
         </is>
       </c>
-      <c r="C6" t="b">
-        <v>1</v>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>54.714955, -113.3085451</t>
+        </is>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -541,12 +568,15 @@
         <v>1</v>
       </c>
       <c r="F6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>40108</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>2015</v>
       </c>
     </row>
@@ -561,11 +591,13 @@
           <t>IAU-001620-1</t>
         </is>
       </c>
-      <c r="C7" t="b">
-        <v>0</v>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>45.7245513, -65.5242192</t>
+        </is>
       </c>
       <c r="D7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -573,10 +605,13 @@
       <c r="F7" t="b">
         <v>1</v>
       </c>
-      <c r="G7">
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>300</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>2015</v>
       </c>
     </row>
@@ -591,22 +626,27 @@
           <t>IAU-001686-1</t>
         </is>
       </c>
-      <c r="C8" t="b">
-        <v>0</v>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>45.3661092, -71.8493905</t>
+        </is>
       </c>
       <c r="D8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
       </c>
       <c r="F8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>2788</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>2015</v>
       </c>
     </row>
@@ -621,22 +661,27 @@
           <t>IAU-001724-1</t>
         </is>
       </c>
-      <c r="C9" t="b">
-        <v>0</v>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>49.8929267, -97.1515364</t>
+        </is>
       </c>
       <c r="D9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9">
         <v>248</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>2015</v>
       </c>
     </row>
@@ -651,22 +696,27 @@
           <t>IAU-001747-1</t>
         </is>
       </c>
-      <c r="C10" t="b">
-        <v>0</v>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>49.845352, -99.962159</t>
+        </is>
       </c>
       <c r="D10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
       </c>
       <c r="F10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>3069</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>2015</v>
       </c>
     </row>
@@ -681,22 +731,27 @@
           <t>IAU-001755-1</t>
         </is>
       </c>
-      <c r="C11" t="b">
-        <v>0</v>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>43.0041849, -81.2827856</t>
+        </is>
       </c>
       <c r="D11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
       </c>
       <c r="F11" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>1255</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>2015</v>
       </c>
     </row>
@@ -711,22 +766,27 @@
           <t>IAU-001770-1</t>
         </is>
       </c>
-      <c r="C12" t="b">
-        <v>0</v>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>49.2499505, -123.0035478</t>
+        </is>
       </c>
       <c r="D12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="b">
         <v>1</v>
       </c>
       <c r="F12" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12">
         <v>40178</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>2015</v>
       </c>
     </row>
@@ -741,8 +801,10 @@
           <t>IAU-001778-1</t>
         </is>
       </c>
-      <c r="C13" t="b">
-        <v>1</v>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>43.1175731, -79.2476925</t>
+        </is>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -751,12 +813,15 @@
         <v>1</v>
       </c>
       <c r="F13" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13">
         <v>18706</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>2015</v>
       </c>
     </row>
@@ -771,22 +836,27 @@
           <t>IAU-001940-1</t>
         </is>
       </c>
-      <c r="C14" t="b">
-        <v>0</v>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>48.4480607, -123.3227003</t>
+        </is>
       </c>
       <c r="D14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
       </c>
-      <c r="G14">
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14">
         <v>8612</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>2015</v>
       </c>
     </row>
@@ -801,8 +871,10 @@
           <t>IAU-001954-1</t>
         </is>
       </c>
-      <c r="C15" t="b">
-        <v>0</v>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>43.8039591, -79.3718778</t>
+        </is>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -811,12 +883,15 @@
         <v>0</v>
       </c>
       <c r="F15" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15">
         <v>703</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>2015</v>
       </c>
     </row>
@@ -831,11 +906,13 @@
           <t>IAU-001955-1</t>
         </is>
       </c>
-      <c r="C16" t="b">
-        <v>0</v>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>49.8600136, -97.2321798</t>
+        </is>
       </c>
       <c r="D16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" t="b">
         <v>1</v>
@@ -843,10 +920,13 @@
       <c r="F16" t="b">
         <v>1</v>
       </c>
-      <c r="G16">
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16">
         <v>1488</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>2015</v>
       </c>
     </row>
@@ -861,22 +941,27 @@
           <t>IAU-001956-1</t>
         </is>
       </c>
-      <c r="C17" t="b">
-        <v>0</v>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>52.488135, -113.7382612</t>
+        </is>
       </c>
       <c r="D17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" t="b">
-        <v>1</v>
-      </c>
-      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17">
         <v>421</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>2015</v>
       </c>
     </row>
@@ -891,16 +976,21 @@
           <t>IAU-001969-1</t>
         </is>
       </c>
-      <c r="C18" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18" t="b">
-        <v>0</v>
-      </c>
-      <c r="G18">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>46.1685256, -60.0921936</t>
+        </is>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18">
         <v>3500</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>2015</v>
       </c>
     </row>
@@ -915,22 +1005,27 @@
           <t>IAU-001973-1</t>
         </is>
       </c>
-      <c r="C19" t="b">
-        <v>0</v>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>49.317754, -123.019085</t>
+        </is>
       </c>
       <c r="D19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
       </c>
-      <c r="G19">
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19">
         <v>6920</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>2015</v>
       </c>
     </row>
@@ -945,8 +1040,10 @@
           <t>IAU-001997-1</t>
         </is>
       </c>
-      <c r="C20" t="b">
-        <v>1</v>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>45.3875812, -75.6960202</t>
+        </is>
       </c>
       <c r="D20" t="b">
         <v>1</v>
@@ -955,12 +1052,15 @@
         <v>1</v>
       </c>
       <c r="F20" t="b">
-        <v>0</v>
-      </c>
-      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20">
         <v>27883</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>2015</v>
       </c>
     </row>
@@ -975,29 +1075,34 @@
           <t>IAU-002055-1</t>
         </is>
       </c>
-      <c r="C21" t="b">
-        <v>0</v>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>43.7355908, -79.2776793</t>
+        </is>
       </c>
       <c r="D21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
       </c>
-      <c r="G21">
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21">
         <v>22866</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>2015</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>La Cité College Of Applied Arts And Technology</t>
+          <t>La Cit�� College Of Applied Arts And Technology</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1005,22 +1110,27 @@
           <t>IAU-002993-1</t>
         </is>
       </c>
-      <c r="C22" t="b">
-        <v>0</v>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>45.4358445, -75.6343254</t>
+        </is>
       </c>
       <c r="D22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
       </c>
-      <c r="G22">
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22">
         <v>3387</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>2015</v>
       </c>
     </row>
@@ -1035,22 +1145,27 @@
           <t>IAU-003046-1</t>
         </is>
       </c>
-      <c r="C23" t="b">
-        <v>0</v>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>49.8895233, -97.1199403</t>
+        </is>
       </c>
       <c r="D23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" t="b">
         <v>1</v>
       </c>
       <c r="F23" t="b">
-        <v>0</v>
-      </c>
-      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23">
         <v>1124</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>2015</v>
       </c>
     </row>
@@ -1065,8 +1180,10 @@
           <t>IAU-003047-1</t>
         </is>
       </c>
-      <c r="C24" t="b">
-        <v>1</v>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>45.4115581, -75.7096195</t>
+        </is>
       </c>
       <c r="D24" t="b">
         <v>1</v>
@@ -1077,10 +1194,13 @@
       <c r="F24" t="b">
         <v>1</v>
       </c>
-      <c r="G24">
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24">
         <v>405</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>2015</v>
       </c>
     </row>
@@ -1095,8 +1215,10 @@
           <t>IAU-003125-1</t>
         </is>
       </c>
-      <c r="C25" t="b">
-        <v>1</v>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>45.4948363, -73.5779128</t>
+        </is>
       </c>
       <c r="D25" t="b">
         <v>1</v>
@@ -1105,12 +1227,15 @@
         <v>1</v>
       </c>
       <c r="F25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25">
         <v>44568</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>2015</v>
       </c>
     </row>
@@ -1125,11 +1250,13 @@
           <t>IAU-003129-1</t>
         </is>
       </c>
-      <c r="C26" t="b">
-        <v>0</v>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>53.56071, -113.4462203</t>
+        </is>
       </c>
       <c r="D26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" t="b">
         <v>1</v>
@@ -1137,10 +1264,13 @@
       <c r="F26" t="b">
         <v>1</v>
       </c>
-      <c r="G26">
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26">
         <v>1986</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>2015</v>
       </c>
     </row>
@@ -1155,22 +1285,27 @@
           <t>IAU-003135-1</t>
         </is>
       </c>
-      <c r="C27" t="b">
-        <v>0</v>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>43.3898652, -80.4047788</t>
+        </is>
       </c>
       <c r="D27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
       </c>
-      <c r="G27">
+      <c r="G27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27">
         <v>11000</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>2015</v>
       </c>
     </row>
@@ -1185,11 +1320,13 @@
           <t>IAU-003340-1</t>
         </is>
       </c>
-      <c r="C28" t="b">
-        <v>0</v>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>46.1346326, -64.8612334</t>
+        </is>
       </c>
       <c r="D28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" t="b">
         <v>1</v>
@@ -1197,10 +1334,13 @@
       <c r="F28" t="b">
         <v>1</v>
       </c>
-      <c r="G28">
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28">
         <v>970</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>2015</v>
       </c>
     </row>
@@ -1215,8 +1355,10 @@
           <t>IAU-003505-3</t>
         </is>
       </c>
-      <c r="C29" t="b">
-        <v>1</v>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>44.6365812, -63.5916555</t>
+        </is>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -1227,7 +1369,10 @@
       <c r="F29" t="b">
         <v>1</v>
       </c>
-      <c r="H29">
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29">
         <v>2015</v>
       </c>
     </row>
@@ -1242,22 +1387,27 @@
           <t>IAU-004480-1</t>
         </is>
       </c>
-      <c r="C30" t="b">
-        <v>0</v>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>49.2675921, -123.0924294</t>
+        </is>
       </c>
       <c r="D30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" t="b">
         <v>1</v>
       </c>
       <c r="F30" t="b">
-        <v>0</v>
-      </c>
-      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30">
         <v>1767</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>2015</v>
       </c>
     </row>
@@ -1272,22 +1422,27 @@
           <t>IAU-006253-1</t>
         </is>
       </c>
-      <c r="C31" t="b">
-        <v>0</v>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>43.0129902, -81.1994209</t>
+        </is>
       </c>
       <c r="D31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
       </c>
-      <c r="G31">
+      <c r="G31" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31">
         <v>18080</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>2015</v>
       </c>
     </row>
@@ -1302,8 +1457,10 @@
           <t>IAU-006615-1</t>
         </is>
       </c>
-      <c r="C32" t="b">
-        <v>0</v>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>43.6760427, -79.4107284</t>
+        </is>
       </c>
       <c r="D32" t="b">
         <v>0</v>
@@ -1314,10 +1471,13 @@
       <c r="F32" t="b">
         <v>0</v>
       </c>
-      <c r="G32">
+      <c r="G32" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32">
         <v>65696</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>2015</v>
       </c>
     </row>
@@ -1332,22 +1492,27 @@
           <t>IAU-006626-1</t>
         </is>
       </c>
-      <c r="C33" t="b">
-        <v>0</v>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>44.4117128, -79.6667919</t>
+        </is>
       </c>
       <c r="D33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
       </c>
-      <c r="G33">
+      <c r="G33" t="b">
+        <v>0</v>
+      </c>
+      <c r="H33">
         <v>11433</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>2015</v>
       </c>
     </row>
@@ -1362,22 +1527,27 @@
           <t>IAU-006768-1</t>
         </is>
       </c>
-      <c r="C34" t="b">
-        <v>0</v>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>53.5470544, -113.506372</t>
+        </is>
       </c>
       <c r="D34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
       </c>
-      <c r="G34">
+      <c r="G34" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34">
         <v>14465</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>2015</v>
       </c>
     </row>
@@ -1392,22 +1562,27 @@
           <t>IAU-007625-1</t>
         </is>
       </c>
-      <c r="C35" t="b">
-        <v>0</v>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>43.7292505, -79.606896</t>
+        </is>
       </c>
       <c r="D35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
       </c>
-      <c r="G35">
+      <c r="G35" t="b">
+        <v>0</v>
+      </c>
+      <c r="H35">
         <v>20600</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <v>2015</v>
       </c>
     </row>
@@ -1422,11 +1597,13 @@
           <t>IAU-007925-1</t>
         </is>
       </c>
-      <c r="C36" t="b">
-        <v>0</v>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>45.4940817, -73.5854666</t>
+        </is>
       </c>
       <c r="D36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36" t="b">
         <v>1</v>
@@ -1434,10 +1611,13 @@
       <c r="F36" t="b">
         <v>1</v>
       </c>
-      <c r="G36">
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36">
         <v>1545</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>2015</v>
       </c>
     </row>
@@ -1452,16 +1632,21 @@
           <t>IAU-008067-1</t>
         </is>
       </c>
-      <c r="C37" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" t="b">
-        <v>0</v>
-      </c>
-      <c r="G37">
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>46.8130236, -71.2240298</t>
+        </is>
+      </c>
+      <c r="D37" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" t="b">
+        <v>0</v>
+      </c>
+      <c r="H37">
         <v>741</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>2015</v>
       </c>
     </row>
@@ -1476,22 +1661,27 @@
           <t>IAU-008327-1</t>
         </is>
       </c>
-      <c r="C38" t="b">
-        <v>1</v>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>43.6613561, -79.3970904</t>
+        </is>
       </c>
       <c r="D38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38" t="b">
         <v>1</v>
       </c>
-      <c r="G38">
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38">
         <v>1995</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <v>2015</v>
       </c>
     </row>
@@ -1506,22 +1696,27 @@
           <t>IAU-010009-1</t>
         </is>
       </c>
-      <c r="C39" t="b">
-        <v>0</v>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>49.2222637, -122.9101326</t>
+        </is>
       </c>
       <c r="D39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
       </c>
-      <c r="G39">
+      <c r="G39" t="b">
+        <v>0</v>
+      </c>
+      <c r="H39">
         <v>28285</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>2015</v>
       </c>
     </row>
@@ -1536,22 +1731,27 @@
           <t>IAU-010661-1</t>
         </is>
       </c>
-      <c r="C40" t="b">
-        <v>0</v>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>49.1332093, -122.8718734</t>
+        </is>
       </c>
       <c r="D40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
       </c>
-      <c r="G40">
+      <c r="G40" t="b">
+        <v>0</v>
+      </c>
+      <c r="H40">
         <v>15119</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>2015</v>
       </c>
     </row>
@@ -1566,8 +1766,10 @@
           <t>IAU-010811-1</t>
         </is>
       </c>
-      <c r="C41" t="b">
-        <v>1</v>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>48.420957, -89.2621479</t>
+        </is>
       </c>
       <c r="D41" t="b">
         <v>1</v>
@@ -1576,12 +1778,15 @@
         <v>1</v>
       </c>
       <c r="F41" t="b">
-        <v>0</v>
-      </c>
-      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="G41" t="b">
+        <v>0</v>
+      </c>
+      <c r="H41">
         <v>7606</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <v>2015</v>
       </c>
     </row>
@@ -1596,30 +1801,34 @@
           <t>IAU-010814-1</t>
         </is>
       </c>
-      <c r="C42" t="b">
-        <v>0</v>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>53.3491288, -110.8728214</t>
+        </is>
       </c>
       <c r="D42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
       </c>
-      <c r="G42">
+      <c r="G42" t="b">
+        <v>0</v>
+      </c>
+      <c r="H42">
         <v>2535</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <v>2015</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Laurentian University
-Huntington University</t>
+          <t>Laurentian University\nHuntington University</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1627,22 +1836,27 @@
           <t>IAU-010871-007656-1</t>
         </is>
       </c>
-      <c r="C43" t="b">
-        <v>0</v>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>46.4642188, -80.9696173</t>
+        </is>
       </c>
       <c r="D43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43" t="b">
         <v>1</v>
       </c>
       <c r="F43" t="b">
-        <v>0</v>
-      </c>
-      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="G43" t="b">
+        <v>0</v>
+      </c>
+      <c r="H43">
         <v>2615</v>
       </c>
-      <c r="H43">
+      <c r="I43">
         <v>2015</v>
       </c>
     </row>
@@ -1657,8 +1871,10 @@
           <t>IAU-010871-2</t>
         </is>
       </c>
-      <c r="C44" t="b">
-        <v>1</v>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>46.4672485, -80.9757296</t>
+        </is>
       </c>
       <c r="D44" t="b">
         <v>1</v>
@@ -1667,9 +1883,12 @@
         <v>1</v>
       </c>
       <c r="F44" t="b">
-        <v>0</v>
-      </c>
-      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="G44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44">
         <v>2015</v>
       </c>
     </row>
@@ -1684,22 +1903,27 @@
           <t>IAU-010917-1</t>
         </is>
       </c>
-      <c r="C45" t="b">
-        <v>0</v>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>49.662341, -112.8089648</t>
+        </is>
       </c>
       <c r="D45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" t="b">
         <v>0</v>
       </c>
-      <c r="G45">
+      <c r="G45" t="b">
+        <v>0</v>
+      </c>
+      <c r="H45">
         <v>4532</v>
       </c>
-      <c r="H45">
+      <c r="I45">
         <v>2015</v>
       </c>
     </row>
@@ -1714,8 +1938,10 @@
           <t>IAU-011496-1</t>
         </is>
       </c>
-      <c r="C46" t="b">
-        <v>1</v>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>45.5047847, -73.5771511</t>
+        </is>
       </c>
       <c r="D46" t="b">
         <v>1</v>
@@ -1724,12 +1950,15 @@
         <v>1</v>
       </c>
       <c r="F46" t="b">
-        <v>0</v>
-      </c>
-      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="G46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H46">
         <v>35356</v>
       </c>
-      <c r="H46">
+      <c r="I46">
         <v>2015</v>
       </c>
     </row>
@@ -1744,11 +1973,13 @@
           <t>IAU-011499-1</t>
         </is>
       </c>
-      <c r="C47" t="b">
-        <v>0</v>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>43.260879, -79.9192254</t>
+        </is>
       </c>
       <c r="D47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47" t="b">
         <v>1</v>
@@ -1756,10 +1987,13 @@
       <c r="F47" t="b">
         <v>1</v>
       </c>
-      <c r="G47">
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47">
         <v>28631</v>
       </c>
-      <c r="H47">
+      <c r="I47">
         <v>2015</v>
       </c>
     </row>
@@ -1774,22 +2008,27 @@
           <t>IAU-011516-1</t>
         </is>
       </c>
-      <c r="C48" t="b">
-        <v>0</v>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>50.0173327, -110.6858492</t>
+        </is>
       </c>
       <c r="D48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48" t="b">
         <v>0</v>
       </c>
-      <c r="G48">
+      <c r="G48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H48">
         <v>2428</v>
       </c>
-      <c r="H48">
+      <c r="I48">
         <v>2015</v>
       </c>
     </row>
@@ -1804,8 +2043,10 @@
           <t>IAU-011558-1</t>
         </is>
       </c>
-      <c r="C49" t="b">
-        <v>1</v>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>47.5737975, -52.7329053</t>
+        </is>
       </c>
       <c r="D49" t="b">
         <v>1</v>
@@ -1814,12 +2055,15 @@
         <v>1</v>
       </c>
       <c r="F49" t="b">
-        <v>0</v>
-      </c>
-      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="G49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H49">
         <v>18694</v>
       </c>
-      <c r="H49">
+      <c r="I49">
         <v>2015</v>
       </c>
     </row>
@@ -1834,11 +2078,13 @@
           <t>IAU-012185-1</t>
         </is>
       </c>
-      <c r="C50" t="b">
-        <v>0</v>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>45.8983184, -64.3731004</t>
+        </is>
       </c>
       <c r="D50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50" t="b">
         <v>1</v>
@@ -1846,10 +2092,13 @@
       <c r="F50" t="b">
         <v>1</v>
       </c>
-      <c r="G50">
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50">
         <v>2303</v>
       </c>
-      <c r="H50">
+      <c r="I50">
         <v>2015</v>
       </c>
     </row>
@@ -1864,22 +2113,27 @@
           <t>IAU-012199-1</t>
         </is>
       </c>
-      <c r="C51" t="b">
-        <v>0</v>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>51.0111361, -114.1318513</t>
+        </is>
       </c>
       <c r="D51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51" t="b">
         <v>0</v>
       </c>
-      <c r="G51">
+      <c r="G51" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51">
         <v>12855</v>
       </c>
-      <c r="H51">
+      <c r="I51">
         <v>2015</v>
       </c>
     </row>
@@ -1894,8 +2148,10 @@
           <t>IAU-012203-1</t>
         </is>
       </c>
-      <c r="C52" t="b">
-        <v>1</v>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>44.6712012, -63.6456043</t>
+        </is>
       </c>
       <c r="D52" t="b">
         <v>1</v>
@@ -1904,12 +2160,15 @@
         <v>1</v>
       </c>
       <c r="F52" t="b">
-        <v>0</v>
-      </c>
-      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+      <c r="H52">
         <v>4075</v>
       </c>
-      <c r="H52">
+      <c r="I52">
         <v>2015</v>
       </c>
     </row>
@@ -1924,22 +2183,27 @@
           <t>IAU-012666-1</t>
         </is>
       </c>
-      <c r="C53" t="b">
-        <v>0</v>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>43.0144419, -79.2623403</t>
+        </is>
       </c>
       <c r="D53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" t="b">
         <v>0</v>
       </c>
-      <c r="G53">
+      <c r="G53" t="b">
+        <v>0</v>
+      </c>
+      <c r="H53">
         <v>20026</v>
       </c>
-      <c r="H53">
+      <c r="I53">
         <v>2015</v>
       </c>
     </row>
@@ -1954,8 +2218,10 @@
           <t>IAU-012719-1</t>
         </is>
       </c>
-      <c r="C54" t="b">
-        <v>1</v>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>46.3410366, -79.4908002</t>
+        </is>
       </c>
       <c r="D54" t="b">
         <v>1</v>
@@ -1964,12 +2230,15 @@
         <v>1</v>
       </c>
       <c r="F54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54">
         <v>4894</v>
       </c>
-      <c r="H54">
+      <c r="I54">
         <v>2015</v>
       </c>
     </row>
@@ -1984,22 +2253,27 @@
           <t>IAU-012786-1</t>
         </is>
       </c>
-      <c r="C55" t="b">
-        <v>0</v>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>49.7105195, -124.9712519</t>
+        </is>
       </c>
       <c r="D55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55" t="b">
         <v>0</v>
       </c>
-      <c r="G55">
+      <c r="G55" t="b">
+        <v>0</v>
+      </c>
+      <c r="H55">
         <v>5553</v>
       </c>
-      <c r="H55">
+      <c r="I55">
         <v>2015</v>
       </c>
     </row>
@@ -2014,22 +2288,27 @@
           <t>IAU-012815-1</t>
         </is>
       </c>
-      <c r="C56" t="b">
-        <v>0</v>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>53.5686303, -113.502326</t>
+        </is>
       </c>
       <c r="D56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F56" t="b">
         <v>0</v>
       </c>
-      <c r="G56">
+      <c r="G56" t="b">
+        <v>0</v>
+      </c>
+      <c r="H56">
         <v>19507</v>
       </c>
-      <c r="H56">
+      <c r="I56">
         <v>2015</v>
       </c>
     </row>
@@ -2044,22 +2323,27 @@
           <t>IAU-012923-1</t>
         </is>
       </c>
-      <c r="C57" t="b">
-        <v>0</v>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>44.6495475, -63.5741584</t>
+        </is>
       </c>
       <c r="D57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57" t="b">
         <v>1</v>
       </c>
       <c r="F57" t="b">
-        <v>0</v>
-      </c>
-      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="G57" t="b">
+        <v>0</v>
+      </c>
+      <c r="H57">
         <v>905</v>
       </c>
-      <c r="H57">
+      <c r="I57">
         <v>2015</v>
       </c>
     </row>
@@ -2074,22 +2358,27 @@
           <t>IAU-013031-1</t>
         </is>
       </c>
-      <c r="C58" t="b">
-        <v>0</v>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>49.940072, -119.3954814</t>
+        </is>
       </c>
       <c r="D58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F58" t="b">
         <v>0</v>
       </c>
-      <c r="G58">
+      <c r="G58" t="b">
+        <v>0</v>
+      </c>
+      <c r="H58">
         <v>7816</v>
       </c>
-      <c r="H58">
+      <c r="I58">
         <v>2015</v>
       </c>
     </row>
@@ -2104,16 +2393,21 @@
           <t>IAU-013054-1</t>
         </is>
       </c>
-      <c r="C59" t="b">
-        <v>0</v>
-      </c>
-      <c r="F59" t="b">
-        <v>0</v>
-      </c>
-      <c r="G59">
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>51.7917335, -114.0955676</t>
+        </is>
+      </c>
+      <c r="D59" t="b">
+        <v>0</v>
+      </c>
+      <c r="G59" t="b">
+        <v>0</v>
+      </c>
+      <c r="H59">
         <v>3342</v>
       </c>
-      <c r="H59">
+      <c r="I59">
         <v>2015</v>
       </c>
     </row>
@@ -2128,22 +2422,27 @@
           <t>IAU-013094-1</t>
         </is>
       </c>
-      <c r="C60" t="b">
-        <v>0</v>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>43.6529936, -79.3912166</t>
+        </is>
       </c>
       <c r="D60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60" t="b">
         <v>1</v>
       </c>
       <c r="F60" t="b">
-        <v>0</v>
-      </c>
-      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="G60" t="b">
+        <v>0</v>
+      </c>
+      <c r="H60">
         <v>4793</v>
       </c>
-      <c r="H60">
+      <c r="I60">
         <v>2015</v>
       </c>
     </row>
@@ -2158,8 +2457,10 @@
           <t>IAU-013766-1</t>
         </is>
       </c>
-      <c r="C61" t="b">
-        <v>1</v>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>49.5020034, -97.0455894</t>
+        </is>
       </c>
       <c r="D61" t="b">
         <v>1</v>
@@ -2170,10 +2471,13 @@
       <c r="F61" t="b">
         <v>1</v>
       </c>
-      <c r="G61">
+      <c r="G61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H61">
         <v>285</v>
       </c>
-      <c r="H61">
+      <c r="I61">
         <v>2015</v>
       </c>
     </row>
@@ -2188,16 +2492,21 @@
           <t>IAU-013841-1</t>
         </is>
       </c>
-      <c r="C62" t="b">
-        <v>0</v>
-      </c>
-      <c r="F62" t="b">
-        <v>0</v>
-      </c>
-      <c r="G62">
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>44.2252795, -76.4951412</t>
+        </is>
+      </c>
+      <c r="D62" t="b">
+        <v>0</v>
+      </c>
+      <c r="G62" t="b">
+        <v>0</v>
+      </c>
+      <c r="H62">
         <v>23295</v>
       </c>
-      <c r="H62">
+      <c r="I62">
         <v>2015</v>
       </c>
     </row>
@@ -2212,22 +2521,27 @@
           <t>IAU-013849-1</t>
         </is>
       </c>
-      <c r="C63" t="b">
-        <v>0</v>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>49.7381913, -123.1004121</t>
+        </is>
       </c>
       <c r="D63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F63" t="b">
-        <v>1</v>
-      </c>
-      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="G63" t="b">
+        <v>1</v>
+      </c>
+      <c r="H63">
         <v>420</v>
       </c>
-      <c r="H63">
+      <c r="I63">
         <v>2015</v>
       </c>
     </row>
@@ -2242,22 +2556,27 @@
           <t>IAU-013935-1</t>
         </is>
       </c>
-      <c r="C64" t="b">
-        <v>0</v>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>52.2464744, -113.827603</t>
+        </is>
       </c>
       <c r="D64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F64" t="b">
         <v>0</v>
       </c>
-      <c r="G64">
+      <c r="G64" t="b">
+        <v>0</v>
+      </c>
+      <c r="H64">
         <v>7500</v>
       </c>
-      <c r="H64">
+      <c r="I64">
         <v>2015</v>
       </c>
     </row>
@@ -2272,22 +2591,27 @@
           <t>IAU-013938-1</t>
         </is>
       </c>
-      <c r="C65" t="b">
-        <v>0</v>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>43.211106, -79.9500438</t>
+        </is>
       </c>
       <c r="D65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E65" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F65" t="b">
-        <v>1</v>
-      </c>
-      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="G65" t="b">
+        <v>1</v>
+      </c>
+      <c r="H65">
         <v>939</v>
       </c>
-      <c r="H65">
+      <c r="I65">
         <v>2015</v>
       </c>
     </row>
@@ -2302,8 +2626,10 @@
           <t>IAU-014124-1</t>
         </is>
       </c>
-      <c r="C66" t="b">
-        <v>1</v>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>44.2338812, -76.4675051</t>
+        </is>
       </c>
       <c r="D66" t="b">
         <v>1</v>
@@ -2312,12 +2638,15 @@
         <v>1</v>
       </c>
       <c r="F66" t="b">
-        <v>0</v>
-      </c>
-      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="G66" t="b">
+        <v>0</v>
+      </c>
+      <c r="H66">
         <v>1797</v>
       </c>
-      <c r="H66">
+      <c r="I66">
         <v>2015</v>
       </c>
     </row>
@@ -2332,8 +2661,10 @@
           <t>IAU-014126-1</t>
         </is>
       </c>
-      <c r="C67" t="b">
-        <v>1</v>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>48.4342047, -123.4739689</t>
+        </is>
       </c>
       <c r="D67" t="b">
         <v>1</v>
@@ -2342,12 +2673,15 @@
         <v>1</v>
       </c>
       <c r="F67" t="b">
-        <v>0</v>
-      </c>
-      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="G67" t="b">
+        <v>0</v>
+      </c>
+      <c r="H67">
         <v>3353</v>
       </c>
-      <c r="H67">
+      <c r="I67">
         <v>2015</v>
       </c>
     </row>
@@ -2362,8 +2696,10 @@
           <t>IAU-014158-1</t>
         </is>
       </c>
-      <c r="C68" t="b">
-        <v>1</v>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>43.6576585, -79.3788017</t>
+        </is>
       </c>
       <c r="D68" t="b">
         <v>1</v>
@@ -2372,12 +2708,15 @@
         <v>1</v>
       </c>
       <c r="F68" t="b">
-        <v>0</v>
-      </c>
-      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="G68" t="b">
+        <v>0</v>
+      </c>
+      <c r="H68">
         <v>33328</v>
       </c>
-      <c r="H68">
+      <c r="I68">
         <v>2015</v>
       </c>
     </row>
@@ -2392,8 +2731,10 @@
           <t>IAU-014271-1</t>
         </is>
       </c>
-      <c r="C69" t="b">
-        <v>1</v>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>44.6313301, -63.581457</t>
+        </is>
       </c>
       <c r="D69" t="b">
         <v>1</v>
@@ -2402,12 +2743,15 @@
         <v>1</v>
       </c>
       <c r="F69" t="b">
-        <v>0</v>
-      </c>
-      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="G69" t="b">
+        <v>0</v>
+      </c>
+      <c r="H69">
         <v>7728</v>
       </c>
-      <c r="H69">
+      <c r="I69">
         <v>2015</v>
       </c>
     </row>
@@ -2422,22 +2766,27 @@
           <t>IAU-015159-1</t>
         </is>
       </c>
-      <c r="C70" t="b">
-        <v>0</v>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>43.7951469, -79.3497467</t>
+        </is>
       </c>
       <c r="D70" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F70" t="b">
         <v>0</v>
       </c>
-      <c r="G70">
+      <c r="G70" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70">
         <v>26384</v>
       </c>
-      <c r="H70">
+      <c r="I70">
         <v>2015</v>
       </c>
     </row>
@@ -2452,22 +2801,27 @@
           <t>IAU-015318-1</t>
         </is>
       </c>
-      <c r="C71" t="b">
-        <v>0</v>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>43.4690663, -79.7000411</t>
+        </is>
       </c>
       <c r="D71" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F71" t="b">
         <v>0</v>
       </c>
-      <c r="G71">
+      <c r="G71" t="b">
+        <v>0</v>
+      </c>
+      <c r="H71">
         <v>16840</v>
       </c>
-      <c r="H71">
+      <c r="I71">
         <v>2015</v>
       </c>
     </row>
@@ -2482,8 +2836,10 @@
           <t>IAU-015440-1</t>
         </is>
       </c>
-      <c r="C72" t="b">
-        <v>1</v>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>49.2780937, -122.9198833</t>
+        </is>
       </c>
       <c r="D72" t="b">
         <v>1</v>
@@ -2492,12 +2848,15 @@
         <v>1</v>
       </c>
       <c r="F72" t="b">
-        <v>0</v>
-      </c>
-      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="G72" t="b">
+        <v>0</v>
+      </c>
+      <c r="H72">
         <v>29673</v>
       </c>
-      <c r="H72">
+      <c r="I72">
         <v>2015</v>
       </c>
     </row>
@@ -2512,22 +2871,27 @@
           <t>IAU-015594-1</t>
         </is>
       </c>
-      <c r="C73" t="b">
-        <v>0</v>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>51.0640894, -114.0885397</t>
+        </is>
       </c>
       <c r="D73" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F73" t="b">
         <v>0</v>
       </c>
-      <c r="G73">
+      <c r="G73" t="b">
+        <v>0</v>
+      </c>
+      <c r="H73">
         <v>12633</v>
       </c>
-      <c r="H73">
+      <c r="I73">
         <v>2015</v>
       </c>
     </row>
@@ -2542,22 +2906,27 @@
           <t>IAU-015743-1</t>
         </is>
       </c>
-      <c r="C74" t="b">
-        <v>0</v>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>45.6177357, -61.9953941</t>
+        </is>
       </c>
       <c r="D74" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E74" t="b">
         <v>1</v>
       </c>
       <c r="F74" t="b">
-        <v>0</v>
-      </c>
-      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="G74" t="b">
+        <v>0</v>
+      </c>
+      <c r="H74">
         <v>4432</v>
       </c>
-      <c r="H74">
+      <c r="I74">
         <v>2015</v>
       </c>
     </row>
@@ -2572,22 +2941,27 @@
           <t>IAU-015746-1</t>
         </is>
       </c>
-      <c r="C75" t="b">
-        <v>0</v>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>43.4693483, -80.5453485</t>
+        </is>
       </c>
       <c r="D75" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E75" t="b">
         <v>1</v>
       </c>
       <c r="F75" t="b">
-        <v>0</v>
-      </c>
-      <c r="G75">
+        <v>1</v>
+      </c>
+      <c r="G75" t="b">
+        <v>0</v>
+      </c>
+      <c r="H75">
         <v>896</v>
       </c>
-      <c r="H75">
+      <c r="I75">
         <v>2015</v>
       </c>
     </row>
@@ -2602,22 +2976,27 @@
           <t>IAU-015759-1</t>
         </is>
       </c>
-      <c r="C76" t="b">
-        <v>0</v>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>44.2234851, -76.5280337</t>
+        </is>
       </c>
       <c r="D76" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E76" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F76" t="b">
-        <v>1</v>
-      </c>
-      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="G76" t="b">
+        <v>1</v>
+      </c>
+      <c r="H76">
         <v>5892</v>
       </c>
-      <c r="H76">
+      <c r="I76">
         <v>2015</v>
       </c>
     </row>
@@ -2632,22 +3011,27 @@
           <t>IAU-015769-1</t>
         </is>
       </c>
-      <c r="C77" t="b">
-        <v>0</v>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>44.6313301, -63.581457</t>
+        </is>
       </c>
       <c r="D77" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E77" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F77" t="b">
-        <v>1</v>
-      </c>
-      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="G77" t="b">
+        <v>1</v>
+      </c>
+      <c r="H77">
         <v>527</v>
       </c>
-      <c r="H77">
+      <c r="I77">
         <v>2015</v>
       </c>
     </row>
@@ -2662,11 +3046,13 @@
           <t>IAU-015791-1</t>
         </is>
       </c>
-      <c r="C78" t="b">
-        <v>0</v>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>45.1929557, -67.2819203</t>
+        </is>
       </c>
       <c r="D78" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E78" t="b">
         <v>1</v>
@@ -2674,10 +3060,13 @@
       <c r="F78" t="b">
         <v>1</v>
       </c>
-      <c r="G78">
+      <c r="G78" t="b">
+        <v>1</v>
+      </c>
+      <c r="H78">
         <v>114</v>
       </c>
-      <c r="H78">
+      <c r="I78">
         <v>2015</v>
       </c>
     </row>
@@ -2692,22 +3081,27 @@
           <t>IAU-016483-1</t>
         </is>
       </c>
-      <c r="C79" t="b">
-        <v>0</v>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>53.5254179, -113.4167524</t>
+        </is>
       </c>
       <c r="D79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F79" t="b">
-        <v>1</v>
-      </c>
-      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="G79" t="b">
+        <v>1</v>
+      </c>
+      <c r="H79">
         <v>789</v>
       </c>
-      <c r="H79">
+      <c r="I79">
         <v>2015</v>
       </c>
     </row>
@@ -2722,8 +3116,10 @@
           <t>IAU-016562-1</t>
         </is>
       </c>
-      <c r="C80" t="b">
-        <v>1</v>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>49.2606052, -123.2459938</t>
+        </is>
       </c>
       <c r="D80" t="b">
         <v>1</v>
@@ -2732,12 +3128,15 @@
         <v>1</v>
       </c>
       <c r="F80" t="b">
-        <v>0</v>
-      </c>
-      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="G80" t="b">
+        <v>0</v>
+      </c>
+      <c r="H80">
         <v>55734</v>
       </c>
-      <c r="H80">
+      <c r="I80">
         <v>2015</v>
       </c>
     </row>
@@ -2752,22 +3151,27 @@
           <t>IAU-016620-1</t>
         </is>
       </c>
-      <c r="C81" t="b">
-        <v>0</v>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>49.8912543, -97.153487</t>
+        </is>
       </c>
       <c r="D81" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E81" t="b">
         <v>1</v>
       </c>
       <c r="F81" t="b">
-        <v>0</v>
-      </c>
-      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="G81" t="b">
+        <v>0</v>
+      </c>
+      <c r="H81">
         <v>9519</v>
       </c>
-      <c r="H81">
+      <c r="I81">
         <v>2015</v>
       </c>
     </row>
@@ -2782,22 +3186,27 @@
           <t>IAU-016643-1</t>
         </is>
       </c>
-      <c r="C82" t="b">
-        <v>0</v>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>50.6705062, -120.365894</t>
+        </is>
       </c>
       <c r="D82" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E82" t="b">
         <v>1</v>
       </c>
       <c r="F82" t="b">
-        <v>0</v>
-      </c>
-      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="G82" t="b">
+        <v>0</v>
+      </c>
+      <c r="H82">
         <v>9715</v>
       </c>
-      <c r="H82">
+      <c r="I82">
         <v>2015</v>
       </c>
     </row>
@@ -2812,8 +3221,10 @@
           <t>IAU-016840-1</t>
         </is>
       </c>
-      <c r="C83" t="b">
-        <v>1</v>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>44.3535934, -78.2958488</t>
+        </is>
       </c>
       <c r="D83" t="b">
         <v>1</v>
@@ -2822,12 +3233,15 @@
         <v>1</v>
       </c>
       <c r="F83" t="b">
-        <v>0</v>
-      </c>
-      <c r="G83">
+        <v>1</v>
+      </c>
+      <c r="G83" t="b">
+        <v>0</v>
+      </c>
+      <c r="H83">
         <v>9397</v>
       </c>
-      <c r="H83">
+      <c r="I83">
         <v>2015</v>
       </c>
     </row>
@@ -2842,11 +3256,13 @@
           <t>IAU-016857-1</t>
         </is>
       </c>
-      <c r="C84" t="b">
-        <v>0</v>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>49.1401752, -122.599982</t>
+        </is>
       </c>
       <c r="D84" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E84" t="b">
         <v>1</v>
@@ -2854,10 +3270,13 @@
       <c r="F84" t="b">
         <v>1</v>
       </c>
-      <c r="G84">
+      <c r="G84" t="b">
+        <v>1</v>
+      </c>
+      <c r="H84">
         <v>3970</v>
       </c>
-      <c r="H84">
+      <c r="I84">
         <v>2015</v>
       </c>
     </row>
@@ -2872,8 +3291,10 @@
           <t>IAU-016965-1</t>
         </is>
       </c>
-      <c r="C85" t="b">
-        <v>1</v>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>43.7971607, -79.3922064</t>
+        </is>
       </c>
       <c r="D85" t="b">
         <v>1</v>
@@ -2884,10 +3305,13 @@
       <c r="F85" t="b">
         <v>1</v>
       </c>
-      <c r="G85">
+      <c r="G85" t="b">
+        <v>1</v>
+      </c>
+      <c r="H85">
         <v>1196</v>
       </c>
-      <c r="H85">
+      <c r="I85">
         <v>2015</v>
       </c>
     </row>
@@ -2902,8 +3326,10 @@
           <t>IAU-019621-1</t>
         </is>
       </c>
-      <c r="C86" t="b">
-        <v>1</v>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>46.1057445, -64.7846855</t>
+        </is>
       </c>
       <c r="D86" t="b">
         <v>1</v>
@@ -2912,20 +3338,22 @@
         <v>1</v>
       </c>
       <c r="F86" t="b">
-        <v>0</v>
-      </c>
-      <c r="G86">
+        <v>1</v>
+      </c>
+      <c r="G86" t="b">
+        <v>0</v>
+      </c>
+      <c r="H86">
         <v>5812</v>
       </c>
-      <c r="H86">
+      <c r="I86">
         <v>2015</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>University Of Montreal
-Polytechnic School Of Montreal</t>
+          <t>University Of Montreal\nPolytechnic School Of Montreal</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2933,8 +3361,10 @@
           <t>IAU-019623-004208-1</t>
         </is>
       </c>
-      <c r="C87" t="b">
-        <v>1</v>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>45.5047939, -73.6131831</t>
+        </is>
       </c>
       <c r="D87" t="b">
         <v>1</v>
@@ -2943,20 +3373,22 @@
         <v>1</v>
       </c>
       <c r="F87" t="b">
-        <v>0</v>
-      </c>
-      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="G87" t="b">
+        <v>0</v>
+      </c>
+      <c r="H87">
         <v>12120</v>
       </c>
-      <c r="H87">
+      <c r="I87">
         <v>2015</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>University Of Montreal
-Hec Montreal</t>
+          <t>University Of Montreal\nHec Montreal</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2964,8 +3396,10 @@
           <t>IAU-019623-007137-1</t>
         </is>
       </c>
-      <c r="C88" t="b">
-        <v>1</v>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>45.5035488, -73.6211175</t>
+        </is>
       </c>
       <c r="D88" t="b">
         <v>1</v>
@@ -2974,12 +3408,15 @@
         <v>1</v>
       </c>
       <c r="F88" t="b">
-        <v>0</v>
-      </c>
-      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="G88" t="b">
+        <v>0</v>
+      </c>
+      <c r="H88">
         <v>47447</v>
       </c>
-      <c r="H88">
+      <c r="I88">
         <v>2015</v>
       </c>
     </row>
@@ -2994,8 +3431,10 @@
           <t>IAU-019623-1</t>
         </is>
       </c>
-      <c r="C89" t="b">
-        <v>1</v>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>45.5056156, -73.6137592</t>
+        </is>
       </c>
       <c r="D89" t="b">
         <v>1</v>
@@ -3004,12 +3443,15 @@
         <v>1</v>
       </c>
       <c r="F89" t="b">
-        <v>0</v>
-      </c>
-      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="G89" t="b">
+        <v>0</v>
+      </c>
+      <c r="H89">
         <v>57696</v>
       </c>
-      <c r="H89">
+      <c r="I89">
         <v>2015</v>
       </c>
     </row>
@@ -3024,8 +3466,10 @@
           <t>IAU-019648-1</t>
         </is>
       </c>
-      <c r="C90" t="b">
-        <v>1</v>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>45.3778253, -71.9292831</t>
+        </is>
       </c>
       <c r="D90" t="b">
         <v>1</v>
@@ -3036,18 +3480,20 @@
       <c r="F90" t="b">
         <v>1</v>
       </c>
-      <c r="G90">
+      <c r="G90" t="b">
+        <v>1</v>
+      </c>
+      <c r="H90">
         <v>37144</v>
       </c>
-      <c r="H90">
+      <c r="I90">
         <v>2015</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>University Of Quebec
-Engineering School - Ets</t>
+          <t>University Of Quebec\nEngineering School - Ets</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -3055,8 +3501,10 @@
           <t>IAU-019700-004020-1</t>
         </is>
       </c>
-      <c r="C91" t="b">
-        <v>1</v>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>46.8138009, -71.2224769</t>
+        </is>
       </c>
       <c r="D91" t="b">
         <v>1</v>
@@ -3065,20 +3513,22 @@
         <v>1</v>
       </c>
       <c r="F91" t="b">
-        <v>0</v>
-      </c>
-      <c r="G91">
+        <v>1</v>
+      </c>
+      <c r="G91" t="b">
+        <v>0</v>
+      </c>
+      <c r="H91">
         <v>7708</v>
       </c>
-      <c r="H91">
+      <c r="I91">
         <v>2015</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>University Of Quebec
-National School Of Public Administration</t>
+          <t>University Of Quebec\nNational School Of Public Administration</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -3086,22 +3536,27 @@
           <t>IAU-019700-004084-1</t>
         </is>
       </c>
-      <c r="C92" t="b">
-        <v>1</v>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>46.8138009, -71.2224769</t>
+        </is>
       </c>
       <c r="D92" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E92" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F92" t="b">
-        <v>0</v>
-      </c>
-      <c r="G92">
+        <v>1</v>
+      </c>
+      <c r="G92" t="b">
+        <v>0</v>
+      </c>
+      <c r="H92">
         <v>5532</v>
       </c>
-      <c r="H92">
+      <c r="I92">
         <v>2015</v>
       </c>
     </row>
@@ -3116,8 +3571,10 @@
           <t>IAU-019700-1</t>
         </is>
       </c>
-      <c r="C93" t="b">
-        <v>1</v>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>46.8132529, -71.2224014</t>
+        </is>
       </c>
       <c r="D93" t="b">
         <v>1</v>
@@ -3126,12 +3583,15 @@
         <v>1</v>
       </c>
       <c r="F93" t="b">
-        <v>0</v>
-      </c>
-      <c r="G93">
+        <v>1</v>
+      </c>
+      <c r="G93" t="b">
+        <v>0</v>
+      </c>
+      <c r="H93">
         <v>90540</v>
       </c>
-      <c r="H93">
+      <c r="I93">
         <v>2015</v>
       </c>
     </row>
@@ -3146,16 +3606,21 @@
           <t>IAU-019701-1</t>
         </is>
       </c>
-      <c r="C94" t="b">
-        <v>1</v>
-      </c>
-      <c r="F94" t="b">
-        <v>0</v>
-      </c>
-      <c r="G94">
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>48.419008, -71.052621</t>
+        </is>
+      </c>
+      <c r="D94" t="b">
+        <v>1</v>
+      </c>
+      <c r="G94" t="b">
+        <v>0</v>
+      </c>
+      <c r="H94">
         <v>351</v>
       </c>
-      <c r="H94">
+      <c r="I94">
         <v>2015</v>
       </c>
     </row>
@@ -3170,16 +3635,21 @@
           <t>IAU-019702-1</t>
         </is>
       </c>
-      <c r="C95" t="b">
-        <v>1</v>
-      </c>
-      <c r="F95" t="b">
-        <v>0</v>
-      </c>
-      <c r="G95">
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>46.8133732, -71.2223552</t>
+        </is>
+      </c>
+      <c r="D95" t="b">
+        <v>1</v>
+      </c>
+      <c r="G95" t="b">
+        <v>0</v>
+      </c>
+      <c r="H95">
         <v>15455</v>
       </c>
-      <c r="H95">
+      <c r="I95">
         <v>2015</v>
       </c>
     </row>
@@ -3194,16 +3664,21 @@
           <t>IAU-019703-1</t>
         </is>
       </c>
-      <c r="C96" t="b">
-        <v>0</v>
-      </c>
-      <c r="F96" t="b">
-        <v>0</v>
-      </c>
-      <c r="G96">
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>45.5125995, -73.5605955</t>
+        </is>
+      </c>
+      <c r="D96" t="b">
+        <v>0</v>
+      </c>
+      <c r="G96" t="b">
+        <v>0</v>
+      </c>
+      <c r="H96">
         <v>47029</v>
       </c>
-      <c r="H96">
+      <c r="I96">
         <v>2015</v>
       </c>
     </row>
@@ -3218,23 +3693,28 @@
           <t>IAU-019704-1</t>
         </is>
       </c>
-      <c r="C97" t="b">
-        <v>1</v>
-      </c>
-      <c r="F97" t="b">
-        <v>0</v>
-      </c>
-      <c r="G97">
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>48.4525603, -68.5121318</t>
+        </is>
+      </c>
+      <c r="D97" t="b">
+        <v>1</v>
+      </c>
+      <c r="G97" t="b">
+        <v>0</v>
+      </c>
+      <c r="H97">
         <v>7128</v>
       </c>
-      <c r="H97">
+      <c r="I97">
         <v>2015</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>University Of Quebec At Trois-RivièRes</t>
+          <t>University Of Quebec At Trois-Rivi��Res</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -3242,16 +3722,21 @@
           <t>IAU-019705-1</t>
         </is>
       </c>
-      <c r="C98" t="b">
-        <v>1</v>
-      </c>
-      <c r="F98" t="b">
-        <v>0</v>
-      </c>
-      <c r="G98">
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>46.3470249, -72.5785097</t>
+        </is>
+      </c>
+      <c r="D98" t="b">
+        <v>1</v>
+      </c>
+      <c r="G98" t="b">
+        <v>0</v>
+      </c>
+      <c r="H98">
         <v>13333</v>
       </c>
-      <c r="H98">
+      <c r="I98">
         <v>2015</v>
       </c>
     </row>
@@ -3266,16 +3751,21 @@
           <t>IAU-019706-1</t>
         </is>
       </c>
-      <c r="C99" t="b">
-        <v>1</v>
-      </c>
-      <c r="F99" t="b">
-        <v>0</v>
-      </c>
-      <c r="G99">
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>48.2305738, -79.0082905</t>
+        </is>
+      </c>
+      <c r="D99" t="b">
+        <v>1</v>
+      </c>
+      <c r="G99" t="b">
+        <v>0</v>
+      </c>
+      <c r="H99">
         <v>4118</v>
       </c>
-      <c r="H99">
+      <c r="I99">
         <v>2015</v>
       </c>
     </row>
@@ -3290,16 +3780,21 @@
           <t>IAU-019707-1</t>
         </is>
       </c>
-      <c r="C100" t="b">
-        <v>1</v>
-      </c>
-      <c r="F100" t="b">
-        <v>0</v>
-      </c>
-      <c r="G100">
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>45.422466, -75.7387016</t>
+        </is>
+      </c>
+      <c r="D100" t="b">
+        <v>1</v>
+      </c>
+      <c r="G100" t="b">
+        <v>0</v>
+      </c>
+      <c r="H100">
         <v>6311</v>
       </c>
-      <c r="H100">
+      <c r="I100">
         <v>2015</v>
       </c>
     </row>
@@ -3314,8 +3809,10 @@
           <t>IAU-019754-1</t>
         </is>
       </c>
-      <c r="C101" t="b">
-        <v>1</v>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>46.7817463, -71.2747424</t>
+        </is>
       </c>
       <c r="D101" t="b">
         <v>1</v>
@@ -3324,12 +3821,15 @@
         <v>1</v>
       </c>
       <c r="F101" t="b">
-        <v>0</v>
-      </c>
-      <c r="G101">
+        <v>1</v>
+      </c>
+      <c r="G101" t="b">
+        <v>0</v>
+      </c>
+      <c r="H101">
         <v>39672</v>
       </c>
-      <c r="H101">
+      <c r="I101">
         <v>2015</v>
       </c>
     </row>
@@ -3344,22 +3844,27 @@
           <t>IAU-019836-1</t>
         </is>
       </c>
-      <c r="C102" t="b">
-        <v>0</v>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>44.3326798, -66.1168753</t>
+        </is>
       </c>
       <c r="D102" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102" t="b">
         <v>1</v>
       </c>
       <c r="F102" t="b">
-        <v>0</v>
-      </c>
-      <c r="G102">
+        <v>1</v>
+      </c>
+      <c r="G102" t="b">
+        <v>0</v>
+      </c>
+      <c r="H102">
         <v>2091</v>
       </c>
-      <c r="H102">
+      <c r="I102">
         <v>2015</v>
       </c>
     </row>
@@ -3374,11 +3879,13 @@
           <t>IAU-019970-1</t>
         </is>
       </c>
-      <c r="C103" t="b">
-        <v>0</v>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>49.2842222, -123.1144438</t>
+        </is>
       </c>
       <c r="D103" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E103" t="b">
         <v>1</v>
@@ -3386,10 +3893,13 @@
       <c r="F103" t="b">
         <v>1</v>
       </c>
-      <c r="G103">
+      <c r="G103" t="b">
+        <v>1</v>
+      </c>
+      <c r="H103">
         <v>2175</v>
       </c>
-      <c r="H103">
+      <c r="I103">
         <v>2015</v>
       </c>
     </row>
@@ -3404,22 +3914,27 @@
           <t>IAU-019985-1</t>
         </is>
       </c>
-      <c r="C104" t="b">
-        <v>0</v>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>53.8193494, -101.2364889</t>
+        </is>
       </c>
       <c r="D104" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E104" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F104" t="b">
         <v>0</v>
       </c>
-      <c r="G104">
+      <c r="G104" t="b">
+        <v>0</v>
+      </c>
+      <c r="H104">
         <v>2400</v>
       </c>
-      <c r="H104">
+      <c r="I104">
         <v>2015</v>
       </c>
     </row>
@@ -3434,8 +3949,10 @@
           <t>IAU-020010-1</t>
         </is>
       </c>
-      <c r="C105" t="b">
-        <v>1</v>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>53.5232189, -113.5263186</t>
+        </is>
       </c>
       <c r="D105" t="b">
         <v>1</v>
@@ -3444,9 +3961,12 @@
         <v>1</v>
       </c>
       <c r="F105" t="b">
-        <v>0</v>
-      </c>
-      <c r="H105">
+        <v>1</v>
+      </c>
+      <c r="G105" t="b">
+        <v>0</v>
+      </c>
+      <c r="I105">
         <v>2015</v>
       </c>
     </row>
@@ -3461,8 +3981,10 @@
           <t>IAU-020053-1</t>
         </is>
       </c>
-      <c r="C106" t="b">
-        <v>1</v>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>51.0775908, -114.140695</t>
+        </is>
       </c>
       <c r="D106" t="b">
         <v>1</v>
@@ -3471,12 +3993,15 @@
         <v>1</v>
       </c>
       <c r="F106" t="b">
-        <v>0</v>
-      </c>
-      <c r="G106">
+        <v>1</v>
+      </c>
+      <c r="G106" t="b">
+        <v>0</v>
+      </c>
+      <c r="H106">
         <v>29214</v>
       </c>
-      <c r="H106">
+      <c r="I106">
         <v>2015</v>
       </c>
     </row>
@@ -3491,8 +4016,10 @@
           <t>IAU-020173-1</t>
         </is>
       </c>
-      <c r="C107" t="b">
-        <v>1</v>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>43.5327217, -80.2261804</t>
+        </is>
       </c>
       <c r="D107" t="b">
         <v>1</v>
@@ -3503,17 +4030,20 @@
       <c r="F107" t="b">
         <v>1</v>
       </c>
-      <c r="G107">
+      <c r="G107" t="b">
+        <v>1</v>
+      </c>
+      <c r="H107">
         <v>24699</v>
       </c>
-      <c r="H107">
+      <c r="I107">
         <v>2015</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>University Of King’S College</t>
+          <t>University Of King���S College</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3521,16 +4051,21 @@
           <t>IAU-020215-1</t>
         </is>
       </c>
-      <c r="C108" t="b">
-        <v>0</v>
-      </c>
-      <c r="F108" t="b">
-        <v>0</v>
-      </c>
-      <c r="G108">
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>44.6377879, -63.5952579</t>
+        </is>
+      </c>
+      <c r="D108" t="b">
+        <v>0</v>
+      </c>
+      <c r="G108" t="b">
+        <v>0</v>
+      </c>
+      <c r="H108">
         <v>1134</v>
       </c>
-      <c r="H108">
+      <c r="I108">
         <v>2015</v>
       </c>
     </row>
@@ -3545,8 +4080,10 @@
           <t>IAU-020225-1</t>
         </is>
       </c>
-      <c r="C109" t="b">
-        <v>1</v>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>49.6786156, -112.8601177</t>
+        </is>
       </c>
       <c r="D109" t="b">
         <v>1</v>
@@ -3555,20 +4092,22 @@
         <v>1</v>
       </c>
       <c r="F109" t="b">
-        <v>0</v>
-      </c>
-      <c r="G109">
+        <v>1</v>
+      </c>
+      <c r="G109" t="b">
+        <v>0</v>
+      </c>
+      <c r="H109">
         <v>8205</v>
       </c>
-      <c r="H109">
+      <c r="I109">
         <v>2015</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>University Of Manitoba
-St. John'S College (University Of Manitoba)</t>
+          <t>University Of Manitoba\nSt. John'S College (University Of Manitoba)</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3576,8 +4115,10 @@
           <t>IAU-020275-015752-1</t>
         </is>
       </c>
-      <c r="C110" t="b">
-        <v>1</v>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>49.8104996, -97.136858</t>
+        </is>
       </c>
       <c r="D110" t="b">
         <v>1</v>
@@ -3586,20 +4127,22 @@
         <v>1</v>
       </c>
       <c r="F110" t="b">
-        <v>0</v>
-      </c>
-      <c r="G110">
+        <v>1</v>
+      </c>
+      <c r="G110" t="b">
+        <v>0</v>
+      </c>
+      <c r="H110">
         <v>27296</v>
       </c>
-      <c r="H110">
+      <c r="I110">
         <v>2015</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>University Of Manitoba
-St. Paul'S College (University Of Manitoba)</t>
+          <t>University Of Manitoba\nSt. Paul'S College (University Of Manitoba)</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3607,8 +4150,10 @@
           <t>IAU-020275-015783-1</t>
         </is>
       </c>
-      <c r="C111" t="b">
-        <v>1</v>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>49.810367, -97.13801</t>
+        </is>
       </c>
       <c r="D111" t="b">
         <v>1</v>
@@ -3617,12 +4162,15 @@
         <v>1</v>
       </c>
       <c r="F111" t="b">
-        <v>0</v>
-      </c>
-      <c r="G111">
+        <v>1</v>
+      </c>
+      <c r="G111" t="b">
+        <v>0</v>
+      </c>
+      <c r="H111">
         <v>3757</v>
       </c>
-      <c r="H111">
+      <c r="I111">
         <v>2015</v>
       </c>
     </row>
@@ -3637,8 +4185,10 @@
           <t>IAU-020275-1</t>
         </is>
       </c>
-      <c r="C112" t="b">
-        <v>1</v>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>49.8075008, -97.1366259</t>
+        </is>
       </c>
       <c r="D112" t="b">
         <v>1</v>
@@ -3647,12 +4197,15 @@
         <v>1</v>
       </c>
       <c r="F112" t="b">
-        <v>0</v>
-      </c>
-      <c r="G112">
+        <v>1</v>
+      </c>
+      <c r="G112" t="b">
+        <v>0</v>
+      </c>
+      <c r="H112">
         <v>29557</v>
       </c>
-      <c r="H112">
+      <c r="I112">
         <v>2015</v>
       </c>
     </row>
@@ -3667,8 +4220,10 @@
           <t>IAU-020328-1</t>
         </is>
       </c>
-      <c r="C113" t="b">
-        <v>1</v>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>45.3063734, -66.085543</t>
+        </is>
       </c>
       <c r="D113" t="b">
         <v>1</v>
@@ -3677,12 +4232,15 @@
         <v>1</v>
       </c>
       <c r="F113" t="b">
-        <v>0</v>
-      </c>
-      <c r="G113">
+        <v>1</v>
+      </c>
+      <c r="G113" t="b">
+        <v>0</v>
+      </c>
+      <c r="H113">
         <v>10372</v>
       </c>
-      <c r="H113">
+      <c r="I113">
         <v>2015</v>
       </c>
     </row>
@@ -3697,8 +4255,10 @@
           <t>IAU-020354-1</t>
         </is>
       </c>
-      <c r="C114" t="b">
-        <v>1</v>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>53.8922034, -122.8133607</t>
+        </is>
       </c>
       <c r="D114" t="b">
         <v>1</v>
@@ -3707,12 +4267,15 @@
         <v>1</v>
       </c>
       <c r="F114" t="b">
-        <v>0</v>
-      </c>
-      <c r="G114">
+        <v>1</v>
+      </c>
+      <c r="G114" t="b">
+        <v>0</v>
+      </c>
+      <c r="H114">
         <v>3839</v>
       </c>
-      <c r="H114">
+      <c r="I114">
         <v>2015</v>
       </c>
     </row>
@@ -3727,8 +4290,10 @@
           <t>IAU-020365-1</t>
         </is>
       </c>
-      <c r="C115" t="b">
-        <v>1</v>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>43.9454711, -78.8967854</t>
+        </is>
       </c>
       <c r="D115" t="b">
         <v>1</v>
@@ -3737,20 +4302,22 @@
         <v>1</v>
       </c>
       <c r="F115" t="b">
-        <v>0</v>
-      </c>
-      <c r="G115">
+        <v>1</v>
+      </c>
+      <c r="G115" t="b">
+        <v>0</v>
+      </c>
+      <c r="H115">
         <v>8794</v>
       </c>
-      <c r="H115">
+      <c r="I115">
         <v>2015</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>University Of Ottawa
-Saint Paul University</t>
+          <t>University Of Ottawa\nSaint Paul University</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -3758,8 +4325,10 @@
           <t>IAU-020369-020368-1</t>
         </is>
       </c>
-      <c r="C116" t="b">
-        <v>1</v>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>45.4078916, -75.676142</t>
+        </is>
       </c>
       <c r="D116" t="b">
         <v>1</v>
@@ -3768,12 +4337,15 @@
         <v>1</v>
       </c>
       <c r="F116" t="b">
-        <v>0</v>
-      </c>
-      <c r="G116">
+        <v>1</v>
+      </c>
+      <c r="G116" t="b">
+        <v>0</v>
+      </c>
+      <c r="H116">
         <v>25773</v>
       </c>
-      <c r="H116">
+      <c r="I116">
         <v>2015</v>
       </c>
     </row>
@@ -3788,8 +4360,10 @@
           <t>IAU-020369-1</t>
         </is>
       </c>
-      <c r="C117" t="b">
-        <v>1</v>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>45.4231064, -75.6831329</t>
+        </is>
       </c>
       <c r="D117" t="b">
         <v>1</v>
@@ -3798,12 +4372,15 @@
         <v>1</v>
       </c>
       <c r="F117" t="b">
-        <v>0</v>
-      </c>
-      <c r="G117">
+        <v>1</v>
+      </c>
+      <c r="G117" t="b">
+        <v>0</v>
+      </c>
+      <c r="H117">
         <v>42003</v>
       </c>
-      <c r="H117">
+      <c r="I117">
         <v>2015</v>
       </c>
     </row>
@@ -3818,8 +4395,10 @@
           <t>IAU-020437-1</t>
         </is>
       </c>
-      <c r="C118" t="b">
-        <v>1</v>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>46.2568931, -63.1389079</t>
+        </is>
       </c>
       <c r="D118" t="b">
         <v>1</v>
@@ -3828,12 +4407,15 @@
         <v>1</v>
       </c>
       <c r="F118" t="b">
-        <v>0</v>
-      </c>
-      <c r="G118">
+        <v>1</v>
+      </c>
+      <c r="G118" t="b">
+        <v>0</v>
+      </c>
+      <c r="H118">
         <v>4322</v>
       </c>
-      <c r="H118">
+      <c r="I118">
         <v>2015</v>
       </c>
     </row>
@@ -3848,8 +4430,10 @@
           <t>IAU-020447-1</t>
         </is>
       </c>
-      <c r="C119" t="b">
-        <v>1</v>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>50.4154542, -104.5878302</t>
+        </is>
       </c>
       <c r="D119" t="b">
         <v>1</v>
@@ -3858,20 +4442,22 @@
         <v>1</v>
       </c>
       <c r="F119" t="b">
-        <v>0</v>
-      </c>
-      <c r="G119">
+        <v>1</v>
+      </c>
+      <c r="G119" t="b">
+        <v>0</v>
+      </c>
+      <c r="H119">
         <v>13448</v>
       </c>
-      <c r="H119">
+      <c r="I119">
         <v>2015</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>University Of Saskatchewan
-Briercrest College And Seminary</t>
+          <t>University Of Saskatchewan\nBriercrest College And Seminary</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -3879,11 +4465,13 @@
           <t>IAU-020476-023022-1</t>
         </is>
       </c>
-      <c r="C120" t="b">
-        <v>0</v>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>50.4565485, -105.8153681</t>
+        </is>
       </c>
       <c r="D120" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E120" t="b">
         <v>1</v>
@@ -3891,10 +4479,13 @@
       <c r="F120" t="b">
         <v>1</v>
       </c>
-      <c r="G120">
+      <c r="G120" t="b">
+        <v>1</v>
+      </c>
+      <c r="H120">
         <v>2176</v>
       </c>
-      <c r="H120">
+      <c r="I120">
         <v>2015</v>
       </c>
     </row>
@@ -3909,8 +4500,10 @@
           <t>IAU-020476-1</t>
         </is>
       </c>
-      <c r="C121" t="b">
-        <v>1</v>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>52.1334003, -106.6313582</t>
+        </is>
       </c>
       <c r="D121" t="b">
         <v>1</v>
@@ -3919,12 +4512,15 @@
         <v>1</v>
       </c>
       <c r="F121" t="b">
-        <v>0</v>
-      </c>
-      <c r="G121">
+        <v>1</v>
+      </c>
+      <c r="G121" t="b">
+        <v>0</v>
+      </c>
+      <c r="H121">
         <v>21450</v>
       </c>
-      <c r="H121">
+      <c r="I121">
         <v>2015</v>
       </c>
     </row>
@@ -3939,30 +4535,34 @@
           <t>IAU-020555-1</t>
         </is>
       </c>
-      <c r="C122" t="b">
-        <v>0</v>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>49.0313016, -122.2858506</t>
+        </is>
       </c>
       <c r="D122" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E122" t="b">
         <v>1</v>
       </c>
       <c r="F122" t="b">
-        <v>0</v>
-      </c>
-      <c r="G122">
+        <v>1</v>
+      </c>
+      <c r="G122" t="b">
+        <v>0</v>
+      </c>
+      <c r="H122">
         <v>14534</v>
       </c>
-      <c r="H122">
+      <c r="I122">
         <v>2015</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>University Of Toronto
-University Of St. Michael'S College</t>
+          <t>University Of Toronto\nUniversity Of St. Michael'S College</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -3970,8 +4570,10 @@
           <t>IAU-020599-020519-1</t>
         </is>
       </c>
-      <c r="C123" t="b">
-        <v>1</v>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>43.6668637, -79.3904846</t>
+        </is>
       </c>
       <c r="D123" t="b">
         <v>1</v>
@@ -3980,20 +4582,22 @@
         <v>1</v>
       </c>
       <c r="F123" t="b">
-        <v>0</v>
-      </c>
-      <c r="G123">
+        <v>1</v>
+      </c>
+      <c r="G123" t="b">
+        <v>0</v>
+      </c>
+      <c r="H123">
         <v>56479</v>
       </c>
-      <c r="H123">
+      <c r="I123">
         <v>2015</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>University Of Toronto
-University Of Trinity College</t>
+          <t>University Of Toronto\nUniversity Of Trinity College</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -4001,8 +4605,10 @@
           <t>IAU-020599-020601-1</t>
         </is>
       </c>
-      <c r="C124" t="b">
-        <v>1</v>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>43.6651758, -79.3956466</t>
+        </is>
       </c>
       <c r="D124" t="b">
         <v>1</v>
@@ -4011,20 +4617,22 @@
         <v>1</v>
       </c>
       <c r="F124" t="b">
-        <v>0</v>
-      </c>
-      <c r="G124">
+        <v>1</v>
+      </c>
+      <c r="G124" t="b">
+        <v>0</v>
+      </c>
+      <c r="H124">
         <v>56479</v>
       </c>
-      <c r="H124">
+      <c r="I124">
         <v>2015</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>University Of Toronto
-Victoria University</t>
+          <t>University Of Toronto\nVictoria University</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -4032,8 +4640,10 @@
           <t>IAU-020599-020869-1</t>
         </is>
       </c>
-      <c r="C125" t="b">
-        <v>1</v>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>48.4634067, -123.3116935</t>
+        </is>
       </c>
       <c r="D125" t="b">
         <v>1</v>
@@ -4042,20 +4652,22 @@
         <v>1</v>
       </c>
       <c r="F125" t="b">
-        <v>0</v>
-      </c>
-      <c r="G125">
+        <v>1</v>
+      </c>
+      <c r="G125" t="b">
+        <v>0</v>
+      </c>
+      <c r="H125">
         <v>56479</v>
       </c>
-      <c r="H125">
+      <c r="I125">
         <v>2015</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>University Of Toronto
-Wycliffe College</t>
+          <t>University Of Toronto\nWycliffe College</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -4063,22 +4675,27 @@
           <t>IAU-020599-021367-1</t>
         </is>
       </c>
-      <c r="C126" t="b">
-        <v>1</v>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>43.6645047, -79.394678</t>
+        </is>
       </c>
       <c r="D126" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E126" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F126" t="b">
-        <v>0</v>
-      </c>
-      <c r="G126">
+        <v>1</v>
+      </c>
+      <c r="G126" t="b">
+        <v>0</v>
+      </c>
+      <c r="H126">
         <v>56479</v>
       </c>
-      <c r="H126">
+      <c r="I126">
         <v>2015</v>
       </c>
     </row>
@@ -4093,8 +4710,10 @@
           <t>IAU-020599-1</t>
         </is>
       </c>
-      <c r="C127" t="b">
-        <v>1</v>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>43.6609086, -79.3959518</t>
+        </is>
       </c>
       <c r="D127" t="b">
         <v>1</v>
@@ -4105,10 +4724,13 @@
       <c r="F127" t="b">
         <v>1</v>
       </c>
-      <c r="G127">
+      <c r="G127" t="b">
+        <v>1</v>
+      </c>
+      <c r="H127">
         <v>78713</v>
       </c>
-      <c r="H127">
+      <c r="I127">
         <v>2015</v>
       </c>
     </row>
@@ -4123,8 +4745,10 @@
           <t>IAU-020613-1</t>
         </is>
       </c>
-      <c r="C128" t="b">
-        <v>1</v>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>48.4634067, -123.3116935</t>
+        </is>
       </c>
       <c r="D128" t="b">
         <v>1</v>
@@ -4133,12 +4757,15 @@
         <v>1</v>
       </c>
       <c r="F128" t="b">
-        <v>0</v>
-      </c>
-      <c r="G128">
+        <v>1</v>
+      </c>
+      <c r="G128" t="b">
+        <v>0</v>
+      </c>
+      <c r="H128">
         <v>20500</v>
       </c>
-      <c r="H128">
+      <c r="I128">
         <v>2015</v>
       </c>
     </row>
@@ -4153,8 +4780,10 @@
           <t>IAU-020623-1</t>
         </is>
       </c>
-      <c r="C129" t="b">
-        <v>1</v>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>43.4722854, -80.5448576</t>
+        </is>
       </c>
       <c r="D129" t="b">
         <v>1</v>
@@ -4163,20 +4792,22 @@
         <v>1</v>
       </c>
       <c r="F129" t="b">
-        <v>0</v>
-      </c>
-      <c r="G129">
+        <v>1</v>
+      </c>
+      <c r="G129" t="b">
+        <v>0</v>
+      </c>
+      <c r="H129">
         <v>34668</v>
       </c>
-      <c r="H129">
+      <c r="I129">
         <v>2015</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>University Of Western Ontario
-Huron University College</t>
+          <t>University Of Western Ontario\nHuron University College</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -4184,22 +4815,27 @@
           <t>IAU-020629-007657-1</t>
         </is>
       </c>
-      <c r="C130" t="b">
-        <v>0</v>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>43.0089768, -81.2777032</t>
+        </is>
       </c>
       <c r="D130" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E130" t="b">
         <v>1</v>
       </c>
       <c r="F130" t="b">
-        <v>0</v>
-      </c>
-      <c r="G130">
+        <v>1</v>
+      </c>
+      <c r="G130" t="b">
+        <v>0</v>
+      </c>
+      <c r="H130">
         <v>35386</v>
       </c>
-      <c r="H130">
+      <c r="I130">
         <v>2015</v>
       </c>
     </row>
@@ -4214,8 +4850,10 @@
           <t>IAU-020629-1</t>
         </is>
       </c>
-      <c r="C131" t="b">
-        <v>1</v>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>43.0095971, -81.2737336</t>
+        </is>
       </c>
       <c r="D131" t="b">
         <v>1</v>
@@ -4224,12 +4862,15 @@
         <v>1</v>
       </c>
       <c r="F131" t="b">
-        <v>0</v>
-      </c>
-      <c r="G131">
+        <v>1</v>
+      </c>
+      <c r="G131" t="b">
+        <v>0</v>
+      </c>
+      <c r="H131">
         <v>30716</v>
       </c>
-      <c r="H131">
+      <c r="I131">
         <v>2015</v>
       </c>
     </row>
@@ -4244,8 +4885,10 @@
           <t>IAU-020639-1</t>
         </is>
       </c>
-      <c r="C132" t="b">
-        <v>1</v>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>42.3043142, -83.066039</t>
+        </is>
       </c>
       <c r="D132" t="b">
         <v>1</v>
@@ -4254,12 +4897,15 @@
         <v>1</v>
       </c>
       <c r="F132" t="b">
-        <v>0</v>
-      </c>
-      <c r="G132">
+        <v>1</v>
+      </c>
+      <c r="G132" t="b">
+        <v>0</v>
+      </c>
+      <c r="H132">
         <v>16148</v>
       </c>
-      <c r="H132">
+      <c r="I132">
         <v>2015</v>
       </c>
     </row>
@@ -4274,22 +4920,27 @@
           <t>IAU-020824-1</t>
         </is>
       </c>
-      <c r="C133" t="b">
-        <v>0</v>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>49.1573024, -123.9664322</t>
+        </is>
       </c>
       <c r="D133" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E133" t="b">
         <v>1</v>
       </c>
       <c r="F133" t="b">
-        <v>0</v>
-      </c>
-      <c r="G133">
+        <v>1</v>
+      </c>
+      <c r="G133" t="b">
+        <v>0</v>
+      </c>
+      <c r="H133">
         <v>15363</v>
       </c>
-      <c r="H133">
+      <c r="I133">
         <v>2015</v>
       </c>
     </row>
@@ -4304,8 +4955,10 @@
           <t>IAU-021264-1</t>
         </is>
       </c>
-      <c r="C134" t="b">
-        <v>1</v>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>43.473851, -80.5274264</t>
+        </is>
       </c>
       <c r="D134" t="b">
         <v>1</v>
@@ -4314,12 +4967,15 @@
         <v>1</v>
       </c>
       <c r="F134" t="b">
-        <v>0</v>
-      </c>
-      <c r="G134">
+        <v>1</v>
+      </c>
+      <c r="G134" t="b">
+        <v>0</v>
+      </c>
+      <c r="H134">
         <v>18588</v>
       </c>
-      <c r="H134">
+      <c r="I134">
         <v>2015</v>
       </c>
     </row>
@@ -4334,8 +4990,10 @@
           <t>IAU-021739-1</t>
         </is>
       </c>
-      <c r="C135" t="b">
-        <v>1</v>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>43.7734535, -79.5018684</t>
+        </is>
       </c>
       <c r="D135" t="b">
         <v>1</v>
@@ -4344,12 +5002,15 @@
         <v>1</v>
       </c>
       <c r="F135" t="b">
-        <v>0</v>
-      </c>
-      <c r="G135">
+        <v>1</v>
+      </c>
+      <c r="G135" t="b">
+        <v>0</v>
+      </c>
+      <c r="H135">
         <v>53146</v>
       </c>
-      <c r="H135">
+      <c r="I135">
         <v>2015</v>
       </c>
     </row>
@@ -4364,11 +5025,13 @@
           <t>IAU-021740-1</t>
         </is>
       </c>
-      <c r="C136" t="b">
-        <v>0</v>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>49.2048667, -122.9102614</t>
+        </is>
       </c>
       <c r="D136" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E136" t="b">
         <v>1</v>
@@ -4376,10 +5039,13 @@
       <c r="F136" t="b">
         <v>1</v>
       </c>
-      <c r="G136">
+      <c r="G136" t="b">
+        <v>1</v>
+      </c>
+      <c r="H136">
         <v>2175</v>
       </c>
-      <c r="H136">
+      <c r="I136">
         <v>2015</v>
       </c>
     </row>
@@ -4394,22 +5060,27 @@
           <t>IAU-022835-1</t>
         </is>
       </c>
-      <c r="C137" t="b">
-        <v>0</v>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>49.2601303, -123.0449951</t>
+        </is>
       </c>
       <c r="D137" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E137" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F137" t="b">
-        <v>1</v>
-      </c>
-      <c r="G137">
+        <v>0</v>
+      </c>
+      <c r="G137" t="b">
+        <v>1</v>
+      </c>
+      <c r="H137">
         <v>1617</v>
       </c>
-      <c r="H137">
+      <c r="I137">
         <v>2015</v>
       </c>
     </row>
@@ -4424,22 +5095,27 @@
           <t>IAU-022840-1</t>
         </is>
       </c>
-      <c r="C138" t="b">
-        <v>0</v>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>49.2620652, -124.7879237</t>
+        </is>
       </c>
       <c r="D138" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E138" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F138" t="b">
-        <v>1</v>
-      </c>
-      <c r="G138">
+        <v>0</v>
+      </c>
+      <c r="G138" t="b">
+        <v>1</v>
+      </c>
+      <c r="H138">
         <v>1622</v>
       </c>
-      <c r="H138">
+      <c r="I138">
         <v>2015</v>
       </c>
     </row>
@@ -4454,22 +5130,27 @@
           <t>IAU-022843-1</t>
         </is>
       </c>
-      <c r="C139" t="b">
-        <v>0</v>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>60.7499735, -135.0967564</t>
+        </is>
       </c>
       <c r="D139" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E139" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F139" t="b">
         <v>0</v>
       </c>
-      <c r="G139">
+      <c r="G139" t="b">
+        <v>0</v>
+      </c>
+      <c r="H139">
         <v>1909</v>
       </c>
-      <c r="H139">
+      <c r="I139">
         <v>2015</v>
       </c>
     </row>
@@ -4484,22 +5165,27 @@
           <t>IAU-022957-1</t>
         </is>
       </c>
-      <c r="C140" t="b">
-        <v>0</v>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>49.2850457, -123.1192174</t>
+        </is>
       </c>
       <c r="D140" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E140" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F140" t="b">
-        <v>1</v>
-      </c>
-      <c r="G140">
+        <v>0</v>
+      </c>
+      <c r="G140" t="b">
+        <v>1</v>
+      </c>
+      <c r="H140">
         <v>1616</v>
       </c>
-      <c r="H140">
+      <c r="I140">
         <v>2015</v>
       </c>
     </row>
@@ -4510,7 +5196,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A136"/>
+  <dimension ref="A1:A137"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5468,6 +6154,13 @@
         </is>
       </c>
     </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Cape Breton University</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>